<commit_message>
updated PDDL knowledge regarding monsters and player stats
</commit_message>
<xml_diff>
--- a/models/wiki_data_manually_entered.xlsx
+++ b/models/wiki_data_manually_entered.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbe28fe5e73b7d58/Code Projects/dcss-ai-wrapper/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E145C3C3-F83B-4A01-A348-EDD056DD7FE8}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B0329386-3706-4463-B728-867BA149168E}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="4425" windowWidth="19830" windowHeight="15435" activeTab="4" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
+    <workbookView xWindow="9225" yWindow="4905" windowWidth="19830" windowHeight="15435" activeTab="2" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="spells" sheetId="1" r:id="rId1"/>
     <sheet name="skills" sheetId="2" r:id="rId2"/>
-    <sheet name="abilities" sheetId="3" r:id="rId3"/>
-    <sheet name="potions_scrolls" sheetId="4" r:id="rId4"/>
-    <sheet name="god" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
+    <sheet name="abilities" sheetId="3" r:id="rId4"/>
+    <sheet name="potions_scrolls" sheetId="4" r:id="rId5"/>
+    <sheet name="god" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1151" uniqueCount="828">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="830">
   <si>
     <t>Icon</t>
   </si>
@@ -2666,6 +2667,12 @@
   </si>
   <si>
     <t>The Shining One, good god of honourable crusades against evil.</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r*2</t>
   </si>
 </sst>
 </file>
@@ -2764,12 +2771,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2789,6 +2790,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10444,32 +10451,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="M1" s="6" t="s">
+      <c r="I1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T1" t="s">
@@ -10477,22 +10484,22 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="6"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="P2" s="10" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="P2" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="8" t="s">
         <v>228</v>
       </c>
       <c r="R2" t="s">
@@ -10526,14 +10533,14 @@
         <v>11</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="N3" t="str">
         <f>LOWER(M3)</f>
         <v>absolute zero</v>
       </c>
-      <c r="O3" s="9" t="str">
+      <c r="O3" s="7" t="str">
         <f>SUBSTITUTE(N3," ","_")</f>
         <v>absolute_zero</v>
       </c>
@@ -10577,14 +10584,14 @@
         <v>14</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N4" t="str">
         <f t="shared" ref="N4:N67" si="0">LOWER(M4)</f>
         <v>agony</v>
       </c>
-      <c r="O4" s="9" t="str">
+      <c r="O4" s="7" t="str">
         <f t="shared" ref="O4:O67" si="1">SUBSTITUTE(N4," ","_")</f>
         <v>agony</v>
       </c>
@@ -10597,7 +10604,7 @@
         <v>1</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" ref="R4:T67" si="4">IF(Q4, _xlfn.CONCAT("(target_based_spell ",P4,")"),_xlfn.CONCAT("(non_target_based_spell ",P4,")"))</f>
+        <f t="shared" ref="R4:R67" si="4">IF(Q4, _xlfn.CONCAT("(target_based_spell ",P4,")"),_xlfn.CONCAT("(non_target_based_spell ",P4,")"))</f>
         <v>(target_based_spell agony)</v>
       </c>
       <c r="T4" t="s">
@@ -10628,14 +10635,14 @@
         <v>18</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" si="0"/>
         <v>airstrike</v>
       </c>
-      <c r="O5" s="9" t="str">
+      <c r="O5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>airstrike</v>
       </c>
@@ -10656,7 +10663,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1">
-      <c r="A6" s="7"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -10675,14 +10682,14 @@
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="4"/>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="0"/>
         <v>alistair's intoxication</v>
       </c>
-      <c r="O6" s="9" t="str">
+      <c r="O6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>alistair's_intoxication</v>
       </c>
@@ -10703,7 +10710,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="45">
-      <c r="A7" s="7"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
@@ -10724,14 +10731,14 @@
         <v>23</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="0"/>
         <v>animate dead</v>
       </c>
-      <c r="O7" s="9" t="str">
+      <c r="O7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>animate_dead</v>
       </c>
@@ -10752,7 +10759,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="15" customHeight="1">
-      <c r="A8" s="7"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -10773,14 +10780,14 @@
         <v>25</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
         <v>animate skeleton</v>
       </c>
-      <c r="O8" s="9" t="str">
+      <c r="O8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>animate_skeleton</v>
       </c>
@@ -10801,7 +10808,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="45">
-      <c r="A9" s="7"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
@@ -10824,14 +10831,14 @@
         <v>28</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="6" t="s">
         <v>26</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="0"/>
         <v>apportation</v>
       </c>
-      <c r="O9" s="9" t="str">
+      <c r="O9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>apportation</v>
       </c>
@@ -10852,7 +10859,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" customHeight="1">
-      <c r="A10" s="7"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
@@ -10873,14 +10880,14 @@
         <v>31</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="6" t="s">
         <v>29</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="0"/>
         <v>aura of abjuration</v>
       </c>
-      <c r="O10" s="9" t="str">
+      <c r="O10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>aura_of_abjuration</v>
       </c>
@@ -10901,7 +10908,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="45">
-      <c r="A11" s="7"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
@@ -10922,14 +10929,14 @@
         <v>34</v>
       </c>
       <c r="I11" s="4"/>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="0"/>
         <v>beastly appendage</v>
       </c>
-      <c r="O11" s="9" t="str">
+      <c r="O11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>beastly_appendage</v>
       </c>
@@ -10950,7 +10957,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1">
-      <c r="A12" s="7"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -10971,14 +10978,14 @@
         <v>36</v>
       </c>
       <c r="I12" s="4"/>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="6" t="s">
         <v>35</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="0"/>
         <v>blade hands</v>
       </c>
-      <c r="O12" s="9" t="str">
+      <c r="O12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>blade_hands</v>
       </c>
@@ -10999,7 +11006,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="75">
-      <c r="A13" s="7"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
@@ -11020,14 +11027,14 @@
         <v>38</v>
       </c>
       <c r="I13" s="4"/>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="6" t="s">
         <v>37</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="0"/>
         <v>blink</v>
       </c>
-      <c r="O13" s="9" t="str">
+      <c r="O13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>blink</v>
       </c>
@@ -11071,14 +11078,14 @@
         <v>41</v>
       </c>
       <c r="I14" s="4"/>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="6" t="s">
         <v>39</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="0"/>
         <v>bolt of magma</v>
       </c>
-      <c r="O14" s="9" t="str">
+      <c r="O14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>bolt_of_magma</v>
       </c>
@@ -11120,14 +11127,14 @@
         <v>25</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="6" t="s">
         <v>42</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
         <v>borgnjor's revivification</v>
       </c>
-      <c r="O15" s="9" t="str">
+      <c r="O15" s="7" t="str">
         <f t="shared" si="1"/>
         <v>borgnjor's_revivification</v>
       </c>
@@ -11171,14 +11178,14 @@
         <v>41</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="6" t="s">
         <v>43</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
         <v>borgnjor's vile clutch</v>
       </c>
-      <c r="O16" s="9" t="str">
+      <c r="O16" s="7" t="str">
         <f t="shared" si="1"/>
         <v>borgnjor's_vile_clutch</v>
       </c>
@@ -11199,7 +11206,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="15" customHeight="1">
-      <c r="A17" s="7"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
@@ -11218,14 +11225,14 @@
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="4"/>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="6" t="s">
         <v>45</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
         <v>call canine familiar</v>
       </c>
-      <c r="O17" s="9" t="str">
+      <c r="O17" s="7" t="str">
         <f t="shared" si="1"/>
         <v>call_canine_familiar</v>
       </c>
@@ -11246,7 +11253,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="30">
-      <c r="A18" s="7"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
@@ -11267,14 +11274,14 @@
         <v>47</v>
       </c>
       <c r="I18" s="4"/>
-      <c r="M18" s="8" t="s">
+      <c r="M18" s="6" t="s">
         <v>46</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
         <v>call imp</v>
       </c>
-      <c r="O18" s="9" t="str">
+      <c r="O18" s="7" t="str">
         <f t="shared" si="1"/>
         <v>call_imp</v>
       </c>
@@ -11295,7 +11302,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" ht="30" customHeight="1">
-      <c r="A19" s="7"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
@@ -11318,14 +11325,14 @@
         <v>50</v>
       </c>
       <c r="I19" s="4"/>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="6" t="s">
         <v>48</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="0"/>
         <v>cause fear</v>
       </c>
-      <c r="O19" s="9" t="str">
+      <c r="O19" s="7" t="str">
         <f t="shared" si="1"/>
         <v>cause_fear</v>
       </c>
@@ -11346,7 +11353,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="45">
-      <c r="A20" s="7"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
@@ -11367,14 +11374,14 @@
         <v>53</v>
       </c>
       <c r="I20" s="4"/>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="6" t="s">
         <v>51</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="0"/>
         <v>chain lightning</v>
       </c>
-      <c r="O20" s="9" t="str">
+      <c r="O20" s="7" t="str">
         <f t="shared" si="1"/>
         <v>chain_lightning</v>
       </c>
@@ -11414,14 +11421,14 @@
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="4"/>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="6" t="s">
         <v>54</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="0"/>
         <v>confusing touch</v>
       </c>
-      <c r="O21" s="9" t="str">
+      <c r="O21" s="7" t="str">
         <f t="shared" si="1"/>
         <v>confusing_touch</v>
       </c>
@@ -11442,7 +11449,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" ht="30" customHeight="1">
-      <c r="A22" s="7"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
@@ -11463,14 +11470,14 @@
         <v>56</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="M22" s="8" t="s">
+      <c r="M22" s="6" t="s">
         <v>55</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="0"/>
         <v>conjure ball lightning</v>
       </c>
-      <c r="O22" s="9" t="str">
+      <c r="O22" s="7" t="str">
         <f t="shared" si="1"/>
         <v>conjure_ball_lightning</v>
       </c>
@@ -11491,7 +11498,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" ht="30">
-      <c r="A23" s="7"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="4" t="s">
         <v>57</v>
       </c>
@@ -11512,14 +11519,14 @@
         <v>18</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="M23" s="8" t="s">
+      <c r="M23" s="6" t="s">
         <v>57</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="0"/>
         <v>conjure flame</v>
       </c>
-      <c r="O23" s="9" t="str">
+      <c r="O23" s="7" t="str">
         <f t="shared" si="1"/>
         <v>conjure_flame</v>
       </c>
@@ -11540,7 +11547,7 @@
       </c>
     </row>
     <row r="24" spans="1:20" ht="15" customHeight="1">
-      <c r="A24" s="7"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
         <v>59</v>
       </c>
@@ -11561,14 +11568,14 @@
         <v>60</v>
       </c>
       <c r="I24" s="4"/>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="6" t="s">
         <v>59</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="0"/>
         <v>controlled blink</v>
       </c>
-      <c r="O24" s="9" t="str">
+      <c r="O24" s="7" t="str">
         <f t="shared" si="1"/>
         <v>controlled_blink</v>
       </c>
@@ -11589,7 +11596,7 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="105">
-      <c r="A25" s="7"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
@@ -11612,14 +11619,14 @@
         <v>14</v>
       </c>
       <c r="I25" s="4"/>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="6" t="s">
         <v>61</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="0"/>
         <v>corona</v>
       </c>
-      <c r="O25" s="9" t="str">
+      <c r="O25" s="7" t="str">
         <f t="shared" si="1"/>
         <v>corona</v>
       </c>
@@ -11640,7 +11647,7 @@
       </c>
     </row>
     <row r="26" spans="1:20" ht="15" customHeight="1">
-      <c r="A26" s="7"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
@@ -11661,14 +11668,14 @@
         <v>63</v>
       </c>
       <c r="I26" s="4"/>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="6" t="s">
         <v>62</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="0"/>
         <v>corpse rot</v>
       </c>
-      <c r="O26" s="9" t="str">
+      <c r="O26" s="7" t="str">
         <f t="shared" si="1"/>
         <v>corpse_rot</v>
       </c>
@@ -11689,7 +11696,7 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="45">
-      <c r="A27" s="7"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
@@ -11712,14 +11719,14 @@
         <v>66</v>
       </c>
       <c r="I27" s="4"/>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="6" t="s">
         <v>64</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="0"/>
         <v>dazzling flash</v>
       </c>
-      <c r="O27" s="9" t="str">
+      <c r="O27" s="7" t="str">
         <f t="shared" si="1"/>
         <v>dazzling_flash</v>
       </c>
@@ -11740,7 +11747,7 @@
       </c>
     </row>
     <row r="28" spans="1:20" ht="15" customHeight="1">
-      <c r="A28" s="7"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>67</v>
       </c>
@@ -11761,14 +11768,14 @@
         <v>68</v>
       </c>
       <c r="I28" s="4"/>
-      <c r="M28" s="8" t="s">
+      <c r="M28" s="6" t="s">
         <v>67</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="0"/>
         <v>death channel</v>
       </c>
-      <c r="O28" s="9" t="str">
+      <c r="O28" s="7" t="str">
         <f t="shared" si="1"/>
         <v>death_channel</v>
       </c>
@@ -11789,7 +11796,7 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="60">
-      <c r="A29" s="7"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
@@ -11810,14 +11817,14 @@
         <v>71</v>
       </c>
       <c r="I29" s="4"/>
-      <c r="M29" s="8" t="s">
+      <c r="M29" s="6" t="s">
         <v>69</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="0"/>
         <v>death's door</v>
       </c>
-      <c r="O29" s="9" t="str">
+      <c r="O29" s="7" t="str">
         <f t="shared" si="1"/>
         <v>death's_door</v>
       </c>
@@ -11838,7 +11845,7 @@
       </c>
     </row>
     <row r="30" spans="1:20" ht="30">
-      <c r="A30" s="7"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
@@ -11859,14 +11866,14 @@
         <v>73</v>
       </c>
       <c r="I30" s="4"/>
-      <c r="M30" s="8" t="s">
+      <c r="M30" s="6" t="s">
         <v>72</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="0"/>
         <v>discord</v>
       </c>
-      <c r="O30" s="9" t="str">
+      <c r="O30" s="7" t="str">
         <f t="shared" si="1"/>
         <v>discord</v>
       </c>
@@ -11908,14 +11915,14 @@
         <v>75</v>
       </c>
       <c r="I31" s="4"/>
-      <c r="M31" s="8" t="s">
+      <c r="M31" s="6" t="s">
         <v>74</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="0"/>
         <v>disjunction</v>
       </c>
-      <c r="O31" s="9" t="str">
+      <c r="O31" s="7" t="str">
         <f t="shared" si="1"/>
         <v>disjunction</v>
       </c>
@@ -11936,7 +11943,7 @@
       </c>
     </row>
     <row r="32" spans="1:20" ht="15" customHeight="1">
-      <c r="A32" s="7"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
@@ -11959,14 +11966,14 @@
         <v>41</v>
       </c>
       <c r="I32" s="4"/>
-      <c r="M32" s="8" t="s">
+      <c r="M32" s="6" t="s">
         <v>76</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="0"/>
         <v>dispel undead</v>
       </c>
-      <c r="O32" s="9" t="str">
+      <c r="O32" s="7" t="str">
         <f t="shared" si="1"/>
         <v>dispel_undead</v>
       </c>
@@ -11987,7 +11994,7 @@
       </c>
     </row>
     <row r="33" spans="1:20" ht="30">
-      <c r="A33" s="7"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="3" t="s">
         <v>77</v>
       </c>
@@ -12010,14 +12017,14 @@
         <v>78</v>
       </c>
       <c r="I33" s="4"/>
-      <c r="M33" s="8" t="s">
+      <c r="M33" s="6" t="s">
         <v>77</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="0"/>
         <v>dispersal</v>
       </c>
-      <c r="O33" s="9" t="str">
+      <c r="O33" s="7" t="str">
         <f t="shared" si="1"/>
         <v>dispersal</v>
       </c>
@@ -12059,14 +12066,14 @@
         <v>36</v>
       </c>
       <c r="I34" s="4"/>
-      <c r="M34" s="8" t="s">
+      <c r="M34" s="6" t="s">
         <v>79</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="0"/>
         <v>dragon form</v>
       </c>
-      <c r="O34" s="9" t="str">
+      <c r="O34" s="7" t="str">
         <f t="shared" si="1"/>
         <v>dragon_form</v>
       </c>
@@ -12087,7 +12094,7 @@
       </c>
     </row>
     <row r="35" spans="1:20" ht="15" customHeight="1">
-      <c r="A35" s="7"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="3" t="s">
         <v>80</v>
       </c>
@@ -12106,14 +12113,14 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="4"/>
-      <c r="M35" s="8" t="s">
+      <c r="M35" s="6" t="s">
         <v>80</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="0"/>
         <v>dragon's call</v>
       </c>
-      <c r="O35" s="9" t="str">
+      <c r="O35" s="7" t="str">
         <f t="shared" si="1"/>
         <v>dragon's_call</v>
       </c>
@@ -12134,7 +12141,7 @@
       </c>
     </row>
     <row r="36" spans="1:20" ht="105">
-      <c r="A36" s="7"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="4" t="s">
         <v>81</v>
       </c>
@@ -12157,14 +12164,14 @@
         <v>14</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="M36" s="8" t="s">
+      <c r="M36" s="6" t="s">
         <v>81</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="0"/>
         <v>ensorcelled hibernation</v>
       </c>
-      <c r="O36" s="9" t="str">
+      <c r="O36" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ensorcelled_hibernation</v>
       </c>
@@ -12185,7 +12192,7 @@
       </c>
     </row>
     <row r="37" spans="1:20" ht="45">
-      <c r="A37" s="7"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>83</v>
       </c>
@@ -12206,14 +12213,14 @@
         <v>56</v>
       </c>
       <c r="I37" s="4"/>
-      <c r="M37" s="8" t="s">
+      <c r="M37" s="6" t="s">
         <v>83</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="0"/>
         <v>eringya's noxious bog</v>
       </c>
-      <c r="O37" s="9" t="str">
+      <c r="O37" s="7" t="str">
         <f t="shared" si="1"/>
         <v>eringya's_noxious_bog</v>
       </c>
@@ -12255,14 +12262,14 @@
         <v>85</v>
       </c>
       <c r="I38" s="4"/>
-      <c r="M38" s="8" t="s">
+      <c r="M38" s="6" t="s">
         <v>84</v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="0"/>
         <v>excruciating wounds</v>
       </c>
-      <c r="O38" s="9" t="str">
+      <c r="O38" s="7" t="str">
         <f t="shared" si="1"/>
         <v>excruciating_wounds</v>
       </c>
@@ -12283,7 +12290,7 @@
       </c>
     </row>
     <row r="39" spans="1:20" ht="15" customHeight="1">
-      <c r="A39" s="7"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="3" t="s">
         <v>86</v>
       </c>
@@ -12306,14 +12313,14 @@
         <v>87</v>
       </c>
       <c r="I39" s="4"/>
-      <c r="M39" s="8" t="s">
+      <c r="M39" s="6" t="s">
         <v>86</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="0"/>
         <v>fire storm</v>
       </c>
-      <c r="O39" s="9" t="str">
+      <c r="O39" s="7" t="str">
         <f t="shared" si="1"/>
         <v>fire_storm</v>
       </c>
@@ -12334,7 +12341,7 @@
       </c>
     </row>
     <row r="40" spans="1:20" ht="60">
-      <c r="A40" s="7"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="4" t="s">
         <v>88</v>
       </c>
@@ -12357,14 +12364,14 @@
         <v>41</v>
       </c>
       <c r="I40" s="4"/>
-      <c r="M40" s="8" t="s">
+      <c r="M40" s="6" t="s">
         <v>88</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="0"/>
         <v>fireball</v>
       </c>
-      <c r="O40" s="9" t="str">
+      <c r="O40" s="7" t="str">
         <f t="shared" si="1"/>
         <v>fireball</v>
       </c>
@@ -12385,7 +12392,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" ht="30">
-      <c r="A41" s="7"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="4" t="s">
         <v>89</v>
       </c>
@@ -12406,14 +12413,14 @@
         <v>56</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="M41" s="8" t="s">
+      <c r="M41" s="6" t="s">
         <v>89</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="0"/>
         <v>foxfire</v>
       </c>
-      <c r="O41" s="9" t="str">
+      <c r="O41" s="7" t="str">
         <f t="shared" si="1"/>
         <v>foxfire</v>
       </c>
@@ -12434,7 +12441,7 @@
       </c>
     </row>
     <row r="42" spans="1:20" ht="30" customHeight="1">
-      <c r="A42" s="7"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
@@ -12457,14 +12464,14 @@
         <v>91</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="M42" s="8" t="s">
+      <c r="M42" s="6" t="s">
         <v>90</v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="0"/>
         <v>freeze</v>
       </c>
-      <c r="O42" s="9" t="str">
+      <c r="O42" s="7" t="str">
         <f t="shared" si="1"/>
         <v>freeze</v>
       </c>
@@ -12485,7 +12492,7 @@
       </c>
     </row>
     <row r="43" spans="1:20" ht="75">
-      <c r="A43" s="7"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="4" t="s">
         <v>92</v>
       </c>
@@ -12508,14 +12515,14 @@
         <v>94</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="M43" s="8" t="s">
+      <c r="M43" s="6" t="s">
         <v>92</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="0"/>
         <v>freezing cloud</v>
       </c>
-      <c r="O43" s="9" t="str">
+      <c r="O43" s="7" t="str">
         <f t="shared" si="1"/>
         <v>freezing_cloud</v>
       </c>
@@ -12536,7 +12543,7 @@
       </c>
     </row>
     <row r="44" spans="1:20" ht="15" customHeight="1">
-      <c r="A44" s="7"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
@@ -12559,14 +12566,14 @@
         <v>66</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="M44" s="8" t="s">
+      <c r="M44" s="6" t="s">
         <v>95</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="0"/>
         <v>frozen ramparts</v>
       </c>
-      <c r="O44" s="9" t="str">
+      <c r="O44" s="7" t="str">
         <f t="shared" si="1"/>
         <v>frozen_ramparts</v>
       </c>
@@ -12587,7 +12594,7 @@
       </c>
     </row>
     <row r="45" spans="1:20" ht="45">
-      <c r="A45" s="7"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="3" t="s">
         <v>96</v>
       </c>
@@ -12610,14 +12617,14 @@
         <v>97</v>
       </c>
       <c r="I45" s="4"/>
-      <c r="M45" s="8" t="s">
+      <c r="M45" s="6" t="s">
         <v>96</v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="0"/>
         <v>fulminant prism</v>
       </c>
-      <c r="O45" s="9" t="str">
+      <c r="O45" s="7" t="str">
         <f t="shared" si="1"/>
         <v>fulminant_prism</v>
       </c>
@@ -12661,14 +12668,14 @@
         <v>99</v>
       </c>
       <c r="I46" s="4"/>
-      <c r="M46" s="8" t="s">
+      <c r="M46" s="6" t="s">
         <v>98</v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="0"/>
         <v>gell's gravitas</v>
       </c>
-      <c r="O46" s="9" t="str">
+      <c r="O46" s="7" t="str">
         <f t="shared" si="1"/>
         <v>gell's_gravitas</v>
       </c>
@@ -12712,14 +12719,14 @@
         <v>53</v>
       </c>
       <c r="I47" s="4"/>
-      <c r="M47" s="8" t="s">
+      <c r="M47" s="6" t="s">
         <v>100</v>
       </c>
       <c r="N47" t="str">
         <f t="shared" si="0"/>
         <v>hailstorm</v>
       </c>
-      <c r="O47" s="9" t="str">
+      <c r="O47" s="7" t="str">
         <f t="shared" si="1"/>
         <v>hailstorm</v>
       </c>
@@ -12763,14 +12770,14 @@
         <v>104</v>
       </c>
       <c r="I48" s="4"/>
-      <c r="M48" s="8" t="s">
+      <c r="M48" s="6" t="s">
         <v>102</v>
       </c>
       <c r="N48" t="str">
         <f t="shared" si="0"/>
         <v>haunt</v>
       </c>
-      <c r="O48" s="9" t="str">
+      <c r="O48" s="7" t="str">
         <f t="shared" si="1"/>
         <v>haunt</v>
       </c>
@@ -12812,14 +12819,14 @@
         <v>36</v>
       </c>
       <c r="I49" s="4"/>
-      <c r="M49" s="8" t="s">
+      <c r="M49" s="6" t="s">
         <v>105</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="0"/>
         <v>hydra form</v>
       </c>
-      <c r="O49" s="9" t="str">
+      <c r="O49" s="7" t="str">
         <f t="shared" si="1"/>
         <v>hydra_form</v>
       </c>
@@ -12861,14 +12868,14 @@
         <v>36</v>
       </c>
       <c r="I50" s="4"/>
-      <c r="M50" s="8" t="s">
+      <c r="M50" s="6" t="s">
         <v>106</v>
       </c>
       <c r="N50" t="str">
         <f t="shared" si="0"/>
         <v>ice form</v>
       </c>
-      <c r="O50" s="9" t="str">
+      <c r="O50" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ice_form</v>
       </c>
@@ -12910,14 +12917,14 @@
         <v>53</v>
       </c>
       <c r="I51" s="4"/>
-      <c r="M51" s="8" t="s">
+      <c r="M51" s="6" t="s">
         <v>108</v>
       </c>
       <c r="N51" t="str">
         <f t="shared" si="0"/>
         <v>ignite poison</v>
       </c>
-      <c r="O51" s="9" t="str">
+      <c r="O51" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ignite_poison</v>
       </c>
@@ -12938,7 +12945,7 @@
       </c>
     </row>
     <row r="52" spans="1:20" ht="15" customHeight="1">
-      <c r="A52" s="7"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="4" t="s">
         <v>110</v>
       </c>
@@ -12959,14 +12966,14 @@
         <v>53</v>
       </c>
       <c r="I52" s="4"/>
-      <c r="M52" s="8" t="s">
+      <c r="M52" s="6" t="s">
         <v>110</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="0"/>
         <v>ignition</v>
       </c>
-      <c r="O52" s="9" t="str">
+      <c r="O52" s="7" t="str">
         <f t="shared" si="1"/>
         <v>ignition</v>
       </c>
@@ -12987,7 +12994,7 @@
       </c>
     </row>
     <row r="53" spans="1:20" ht="30">
-      <c r="A53" s="7"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="3" t="s">
         <v>112</v>
       </c>
@@ -13010,14 +13017,14 @@
         <v>113</v>
       </c>
       <c r="I53" s="4"/>
-      <c r="M53" s="8" t="s">
+      <c r="M53" s="6" t="s">
         <v>112</v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="0"/>
         <v>infestation</v>
       </c>
-      <c r="O53" s="9" t="str">
+      <c r="O53" s="7" t="str">
         <f t="shared" si="1"/>
         <v>infestation</v>
       </c>
@@ -13059,14 +13066,14 @@
         <v>25</v>
       </c>
       <c r="I54" s="4"/>
-      <c r="M54" s="8" t="s">
+      <c r="M54" s="6" t="s">
         <v>114</v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="0"/>
         <v>infusion</v>
       </c>
-      <c r="O54" s="9" t="str">
+      <c r="O54" s="7" t="str">
         <f t="shared" si="1"/>
         <v>infusion</v>
       </c>
@@ -13087,7 +13094,7 @@
       </c>
     </row>
     <row r="55" spans="1:20" ht="60" customHeight="1">
-      <c r="A55" s="7"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="4" t="s">
         <v>116</v>
       </c>
@@ -13110,14 +13117,14 @@
         <v>118</v>
       </c>
       <c r="I55" s="4"/>
-      <c r="M55" s="8" t="s">
+      <c r="M55" s="6" t="s">
         <v>116</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="0"/>
         <v>inner flame</v>
       </c>
-      <c r="O55" s="9" t="str">
+      <c r="O55" s="7" t="str">
         <f t="shared" si="1"/>
         <v>inner_flame</v>
       </c>
@@ -13138,7 +13145,7 @@
       </c>
     </row>
     <row r="56" spans="1:20" ht="120">
-      <c r="A56" s="7"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="4" t="s">
         <v>119</v>
       </c>
@@ -13161,14 +13168,14 @@
         <v>120</v>
       </c>
       <c r="I56" s="4"/>
-      <c r="M56" s="8" t="s">
+      <c r="M56" s="6" t="s">
         <v>119</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="0"/>
         <v>invisibility</v>
       </c>
-      <c r="O56" s="9" t="str">
+      <c r="O56" s="7" t="str">
         <f t="shared" si="1"/>
         <v>invisibility</v>
       </c>
@@ -13189,7 +13196,7 @@
       </c>
     </row>
     <row r="57" spans="1:20" ht="30" customHeight="1">
-      <c r="A57" s="7"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="4" t="s">
         <v>121</v>
       </c>
@@ -13212,14 +13219,14 @@
         <v>41</v>
       </c>
       <c r="I57" s="4"/>
-      <c r="M57" s="8" t="s">
+      <c r="M57" s="6" t="s">
         <v>121</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="0"/>
         <v>iron shot</v>
       </c>
-      <c r="O57" s="9" t="str">
+      <c r="O57" s="7" t="str">
         <f t="shared" si="1"/>
         <v>iron_shot</v>
       </c>
@@ -13240,7 +13247,7 @@
       </c>
     </row>
     <row r="58" spans="1:20" ht="45">
-      <c r="A58" s="7"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="4" t="s">
         <v>123</v>
       </c>
@@ -13263,14 +13270,14 @@
         <v>125</v>
       </c>
       <c r="I58" s="4"/>
-      <c r="M58" s="8" t="s">
+      <c r="M58" s="6" t="s">
         <v>123</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="0"/>
         <v>irradiate</v>
       </c>
-      <c r="O58" s="9" t="str">
+      <c r="O58" s="7" t="str">
         <f t="shared" si="1"/>
         <v>irradiate</v>
       </c>
@@ -13312,14 +13319,14 @@
         <v>25</v>
       </c>
       <c r="I59" s="4"/>
-      <c r="M59" s="8" t="s">
+      <c r="M59" s="6" t="s">
         <v>126</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="0"/>
         <v>iskenderun's battlesphere</v>
       </c>
-      <c r="O59" s="9" t="str">
+      <c r="O59" s="7" t="str">
         <f t="shared" si="1"/>
         <v>iskenderun's_battlesphere</v>
       </c>
@@ -13363,14 +13370,14 @@
         <v>53</v>
       </c>
       <c r="I60" s="4"/>
-      <c r="M60" s="8" t="s">
+      <c r="M60" s="6" t="s">
         <v>128</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="0"/>
         <v>iskenderun's mystic blast</v>
       </c>
-      <c r="O60" s="9" t="str">
+      <c r="O60" s="7" t="str">
         <f t="shared" si="1"/>
         <v>iskenderun's_mystic_blast</v>
       </c>
@@ -13391,7 +13398,7 @@
       </c>
     </row>
     <row r="61" spans="1:20" ht="30" customHeight="1">
-      <c r="A61" s="7"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="4" t="s">
         <v>130</v>
       </c>
@@ -13412,14 +13419,14 @@
         <v>53</v>
       </c>
       <c r="I61" s="4"/>
-      <c r="M61" s="8" t="s">
+      <c r="M61" s="6" t="s">
         <v>130</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="0"/>
         <v>leda's liquefaction</v>
       </c>
-      <c r="O61" s="9" t="str">
+      <c r="O61" s="7" t="str">
         <f t="shared" si="1"/>
         <v>leda's_liquefaction</v>
       </c>
@@ -13440,7 +13447,7 @@
       </c>
     </row>
     <row r="62" spans="1:20" ht="60">
-      <c r="A62" s="7"/>
+      <c r="A62" s="15"/>
       <c r="B62" s="4" t="s">
         <v>132</v>
       </c>
@@ -13463,14 +13470,14 @@
         <v>134</v>
       </c>
       <c r="I62" s="4"/>
-      <c r="M62" s="8" t="s">
+      <c r="M62" s="6" t="s">
         <v>132</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="0"/>
         <v>lee's rapid deconstruction</v>
       </c>
-      <c r="O62" s="9" t="str">
+      <c r="O62" s="7" t="str">
         <f t="shared" si="1"/>
         <v>lee's_rapid_deconstruction</v>
       </c>
@@ -13491,7 +13498,7 @@
       </c>
     </row>
     <row r="63" spans="1:20" ht="15" customHeight="1">
-      <c r="A63" s="7"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="3" t="s">
         <v>135</v>
       </c>
@@ -13514,14 +13521,14 @@
         <v>41</v>
       </c>
       <c r="I63" s="4"/>
-      <c r="M63" s="8" t="s">
+      <c r="M63" s="6" t="s">
         <v>135</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="0"/>
         <v>lehudib's crystal spear</v>
       </c>
-      <c r="O63" s="9" t="str">
+      <c r="O63" s="7" t="str">
         <f t="shared" si="1"/>
         <v>lehudib's_crystal_spear</v>
       </c>
@@ -13542,7 +13549,7 @@
       </c>
     </row>
     <row r="64" spans="1:20" ht="75">
-      <c r="A64" s="7"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="4" t="s">
         <v>136</v>
       </c>
@@ -13565,14 +13572,14 @@
         <v>137</v>
       </c>
       <c r="I64" s="4"/>
-      <c r="M64" s="8" t="s">
+      <c r="M64" s="6" t="s">
         <v>136</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="0"/>
         <v>lesser beckoning</v>
       </c>
-      <c r="O64" s="9" t="str">
+      <c r="O64" s="7" t="str">
         <f t="shared" si="1"/>
         <v>lesser_beckoning</v>
       </c>
@@ -13616,14 +13623,14 @@
         <v>41</v>
       </c>
       <c r="I65" s="4"/>
-      <c r="M65" s="8" t="s">
+      <c r="M65" s="6" t="s">
         <v>138</v>
       </c>
       <c r="N65" t="str">
         <f t="shared" si="0"/>
         <v>lightning bolt</v>
       </c>
-      <c r="O65" s="9" t="str">
+      <c r="O65" s="7" t="str">
         <f t="shared" si="1"/>
         <v>lightning_bolt</v>
       </c>
@@ -13644,7 +13651,7 @@
       </c>
     </row>
     <row r="66" spans="1:20" ht="45" customHeight="1">
-      <c r="A66" s="7"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="4" t="s">
         <v>139</v>
       </c>
@@ -13667,14 +13674,14 @@
         <v>41</v>
       </c>
       <c r="I66" s="4"/>
-      <c r="M66" s="8" t="s">
+      <c r="M66" s="6" t="s">
         <v>139</v>
       </c>
       <c r="N66" t="str">
         <f t="shared" si="0"/>
         <v>magic dart</v>
       </c>
-      <c r="O66" s="9" t="str">
+      <c r="O66" s="7" t="str">
         <f t="shared" si="1"/>
         <v>magic_dart</v>
       </c>
@@ -13695,7 +13702,7 @@
       </c>
     </row>
     <row r="67" spans="1:20" ht="45">
-      <c r="A67" s="7"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="3" t="s">
         <v>141</v>
       </c>
@@ -13716,14 +13723,14 @@
         <v>143</v>
       </c>
       <c r="I67" s="4"/>
-      <c r="M67" s="8" t="s">
+      <c r="M67" s="6" t="s">
         <v>141</v>
       </c>
       <c r="N67" t="str">
         <f t="shared" si="0"/>
         <v>malign gateway</v>
       </c>
-      <c r="O67" s="9" t="str">
+      <c r="O67" s="7" t="str">
         <f t="shared" si="1"/>
         <v>malign_gateway</v>
       </c>
@@ -13767,14 +13774,14 @@
         <v>146</v>
       </c>
       <c r="I68" s="4"/>
-      <c r="M68" s="8" t="s">
+      <c r="M68" s="6" t="s">
         <v>144</v>
       </c>
       <c r="N68" t="str">
         <f t="shared" ref="N68:N120" si="5">LOWER(M68)</f>
         <v>mephitic cloud</v>
       </c>
-      <c r="O68" s="9" t="str">
+      <c r="O68" s="7" t="str">
         <f t="shared" ref="O68:O120" si="6">SUBSTITUTE(N68," ","_")</f>
         <v>mephitic_cloud</v>
       </c>
@@ -13787,7 +13794,7 @@
         <v>1</v>
       </c>
       <c r="R68" t="str">
-        <f t="shared" ref="R68:T120" si="9">IF(Q68, _xlfn.CONCAT("(target_based_spell ",P68,")"),_xlfn.CONCAT("(non_target_based_spell ",P68,")"))</f>
+        <f t="shared" ref="R68:R120" si="9">IF(Q68, _xlfn.CONCAT("(target_based_spell ",P68,")"),_xlfn.CONCAT("(non_target_based_spell ",P68,")"))</f>
         <v>(target_based_spell mephitic_cloud)</v>
       </c>
       <c r="T68" t="s">
@@ -13816,14 +13823,14 @@
         <v>53</v>
       </c>
       <c r="I69" s="4"/>
-      <c r="M69" s="8" t="s">
+      <c r="M69" s="6" t="s">
         <v>147</v>
       </c>
       <c r="N69" t="str">
         <f t="shared" si="5"/>
         <v>metabolic englaciation</v>
       </c>
-      <c r="O69" s="9" t="str">
+      <c r="O69" s="7" t="str">
         <f t="shared" si="6"/>
         <v>metabolic_englaciation</v>
       </c>
@@ -13844,7 +13851,7 @@
       </c>
     </row>
     <row r="70" spans="1:20" ht="15" customHeight="1">
-      <c r="A70" s="7"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="3" t="s">
         <v>148</v>
       </c>
@@ -13865,14 +13872,14 @@
         <v>149</v>
       </c>
       <c r="I70" s="4"/>
-      <c r="M70" s="8" t="s">
+      <c r="M70" s="6" t="s">
         <v>148</v>
       </c>
       <c r="N70" t="str">
         <f t="shared" si="5"/>
         <v>monstrous menagerie</v>
       </c>
-      <c r="O70" s="9" t="str">
+      <c r="O70" s="7" t="str">
         <f t="shared" si="6"/>
         <v>monstrous_menagerie</v>
       </c>
@@ -13893,7 +13900,7 @@
       </c>
     </row>
     <row r="71" spans="1:20" ht="60">
-      <c r="A71" s="7"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="3" t="s">
         <v>150</v>
       </c>
@@ -13914,14 +13921,14 @@
         <v>34</v>
       </c>
       <c r="I71" s="4"/>
-      <c r="M71" s="8" t="s">
+      <c r="M71" s="6" t="s">
         <v>150</v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="5"/>
         <v>necromutation</v>
       </c>
-      <c r="O71" s="9" t="str">
+      <c r="O71" s="7" t="str">
         <f t="shared" si="6"/>
         <v>necromutation</v>
       </c>
@@ -13942,7 +13949,7 @@
       </c>
     </row>
     <row r="72" spans="1:20" ht="60">
-      <c r="A72" s="7"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="3" t="s">
         <v>152</v>
       </c>
@@ -13963,14 +13970,14 @@
         <v>53</v>
       </c>
       <c r="I72" s="4"/>
-      <c r="M72" s="8" t="s">
+      <c r="M72" s="6" t="s">
         <v>152</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="5"/>
         <v>olgreb's toxic radiance</v>
       </c>
-      <c r="O72" s="9" t="str">
+      <c r="O72" s="7" t="str">
         <f t="shared" si="6"/>
         <v>olgreb's_toxic_radiance</v>
       </c>
@@ -14014,14 +14021,14 @@
         <v>137</v>
       </c>
       <c r="I73" s="4"/>
-      <c r="M73" s="8" t="s">
+      <c r="M73" s="6" t="s">
         <v>154</v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="5"/>
         <v>orb of destruction</v>
       </c>
-      <c r="O73" s="9" t="str">
+      <c r="O73" s="7" t="str">
         <f t="shared" si="6"/>
         <v>orb_of_destruction</v>
       </c>
@@ -14063,14 +14070,14 @@
         <v>11</v>
       </c>
       <c r="I74" s="4"/>
-      <c r="M74" s="8" t="s">
+      <c r="M74" s="6" t="s">
         <v>155</v>
       </c>
       <c r="N74" t="str">
         <f t="shared" si="5"/>
         <v>ozocubu's armour</v>
       </c>
-      <c r="O74" s="9" t="str">
+      <c r="O74" s="7" t="str">
         <f t="shared" si="6"/>
         <v>ozocubu's_armour</v>
       </c>
@@ -14091,7 +14098,7 @@
       </c>
     </row>
     <row r="75" spans="1:20" ht="15" customHeight="1">
-      <c r="A75" s="7"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="3" t="s">
         <v>157</v>
       </c>
@@ -14112,14 +14119,14 @@
         <v>53</v>
       </c>
       <c r="I75" s="4"/>
-      <c r="M75" s="8" t="s">
+      <c r="M75" s="6" t="s">
         <v>157</v>
       </c>
       <c r="N75" t="str">
         <f t="shared" si="5"/>
         <v>ozocubu's refrigeration</v>
       </c>
-      <c r="O75" s="9" t="str">
+      <c r="O75" s="7" t="str">
         <f t="shared" si="6"/>
         <v>ozocubu's_refrigeration</v>
       </c>
@@ -14140,7 +14147,7 @@
       </c>
     </row>
     <row r="76" spans="1:20" ht="90">
-      <c r="A76" s="7"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="3" t="s">
         <v>158</v>
       </c>
@@ -14163,14 +14170,14 @@
         <v>159</v>
       </c>
       <c r="I76" s="4"/>
-      <c r="M76" s="8" t="s">
+      <c r="M76" s="6" t="s">
         <v>158</v>
       </c>
       <c r="N76" t="str">
         <f t="shared" si="5"/>
         <v>pain</v>
       </c>
-      <c r="O76" s="9" t="str">
+      <c r="O76" s="7" t="str">
         <f t="shared" si="6"/>
         <v>pain</v>
       </c>
@@ -14191,7 +14198,7 @@
       </c>
     </row>
     <row r="77" spans="1:20" ht="15" customHeight="1">
-      <c r="A77" s="7"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="4" t="s">
         <v>160</v>
       </c>
@@ -14214,14 +14221,14 @@
         <v>161</v>
       </c>
       <c r="I77" s="4"/>
-      <c r="M77" s="8" t="s">
+      <c r="M77" s="6" t="s">
         <v>160</v>
       </c>
       <c r="N77" t="str">
         <f t="shared" si="5"/>
         <v>passage of golubria</v>
       </c>
-      <c r="O77" s="9" t="str">
+      <c r="O77" s="7" t="str">
         <f t="shared" si="6"/>
         <v>passage_of_golubria</v>
       </c>
@@ -14242,7 +14249,7 @@
       </c>
     </row>
     <row r="78" spans="1:20" ht="60">
-      <c r="A78" s="7"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="4" t="s">
         <v>162</v>
       </c>
@@ -14265,14 +14272,14 @@
         <v>164</v>
       </c>
       <c r="I78" s="4"/>
-      <c r="M78" s="8" t="s">
+      <c r="M78" s="6" t="s">
         <v>162</v>
       </c>
       <c r="N78" t="str">
         <f t="shared" si="5"/>
         <v>passwall</v>
       </c>
-      <c r="O78" s="9" t="str">
+      <c r="O78" s="7" t="str">
         <f t="shared" si="6"/>
         <v>passwall</v>
       </c>
@@ -14293,7 +14300,7 @@
       </c>
     </row>
     <row r="79" spans="1:20" ht="15" customHeight="1">
-      <c r="A79" s="7"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="4" t="s">
         <v>165</v>
       </c>
@@ -14316,14 +14323,14 @@
         <v>159</v>
       </c>
       <c r="I79" s="4"/>
-      <c r="M79" s="8" t="s">
+      <c r="M79" s="6" t="s">
         <v>165</v>
       </c>
       <c r="N79" t="str">
         <f t="shared" si="5"/>
         <v>petrify</v>
       </c>
-      <c r="O79" s="9" t="str">
+      <c r="O79" s="7" t="str">
         <f t="shared" si="6"/>
         <v>petrify</v>
       </c>
@@ -14344,7 +14351,7 @@
       </c>
     </row>
     <row r="80" spans="1:20" ht="45">
-      <c r="A80" s="7"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="4" t="s">
         <v>166</v>
       </c>
@@ -14367,14 +14374,14 @@
         <v>18</v>
       </c>
       <c r="I80" s="4"/>
-      <c r="M80" s="8" t="s">
+      <c r="M80" s="6" t="s">
         <v>166</v>
       </c>
       <c r="N80" t="str">
         <f t="shared" si="5"/>
         <v>poisonous vapours</v>
       </c>
-      <c r="O80" s="9" t="str">
+      <c r="O80" s="7" t="str">
         <f t="shared" si="6"/>
         <v>poisonous_vapours</v>
       </c>
@@ -14395,7 +14402,7 @@
       </c>
     </row>
     <row r="81" spans="1:20" ht="45">
-      <c r="A81" s="7"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="4" t="s">
         <v>168</v>
       </c>
@@ -14414,14 +14421,14 @@
       </c>
       <c r="H81" s="2"/>
       <c r="I81" s="4"/>
-      <c r="M81" s="8" t="s">
+      <c r="M81" s="6" t="s">
         <v>168</v>
       </c>
       <c r="N81" t="str">
         <f t="shared" si="5"/>
         <v>portal projectile</v>
       </c>
-      <c r="O81" s="9" t="str">
+      <c r="O81" s="7" t="str">
         <f t="shared" si="6"/>
         <v>portal_projectile</v>
       </c>
@@ -14442,7 +14449,7 @@
       </c>
     </row>
     <row r="82" spans="1:20" ht="45">
-      <c r="A82" s="7"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="4" t="s">
         <v>170</v>
       </c>
@@ -14463,14 +14470,14 @@
         <v>25</v>
       </c>
       <c r="I82" s="4"/>
-      <c r="M82" s="8" t="s">
+      <c r="M82" s="6" t="s">
         <v>170</v>
       </c>
       <c r="N82" t="str">
         <f t="shared" si="5"/>
         <v>recall</v>
       </c>
-      <c r="O82" s="9" t="str">
+      <c r="O82" s="7" t="str">
         <f t="shared" si="6"/>
         <v>recall</v>
       </c>
@@ -14491,7 +14498,7 @@
       </c>
     </row>
     <row r="83" spans="1:20" ht="30">
-      <c r="A83" s="7"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="4" t="s">
         <v>171</v>
       </c>
@@ -14512,14 +14519,14 @@
         <v>53</v>
       </c>
       <c r="I83" s="4"/>
-      <c r="M83" s="8" t="s">
+      <c r="M83" s="6" t="s">
         <v>171</v>
       </c>
       <c r="N83" t="str">
         <f t="shared" si="5"/>
         <v>ring of flames</v>
       </c>
-      <c r="O83" s="9" t="str">
+      <c r="O83" s="7" t="str">
         <f t="shared" si="6"/>
         <v>ring_of_flames</v>
       </c>
@@ -14563,14 +14570,14 @@
         <v>137</v>
       </c>
       <c r="I84" s="4"/>
-      <c r="M84" s="8" t="s">
+      <c r="M84" s="6" t="s">
         <v>173</v>
       </c>
       <c r="N84" t="str">
         <f t="shared" si="5"/>
         <v>sandblast</v>
       </c>
-      <c r="O84" s="9" t="str">
+      <c r="O84" s="7" t="str">
         <f t="shared" si="6"/>
         <v>sandblast</v>
       </c>
@@ -14614,14 +14621,14 @@
         <v>41</v>
       </c>
       <c r="I85" s="4"/>
-      <c r="M85" s="8" t="s">
+      <c r="M85" s="6" t="s">
         <v>174</v>
       </c>
       <c r="N85" t="str">
         <f t="shared" si="5"/>
         <v>searing ray</v>
       </c>
-      <c r="O85" s="9" t="str">
+      <c r="O85" s="7" t="str">
         <f t="shared" si="6"/>
         <v>searing_ray</v>
       </c>
@@ -14642,7 +14649,7 @@
       </c>
     </row>
     <row r="86" spans="1:20" ht="60" customHeight="1">
-      <c r="A86" s="7"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="4" t="s">
         <v>175</v>
       </c>
@@ -14663,14 +14670,14 @@
         <v>149</v>
       </c>
       <c r="I86" s="4"/>
-      <c r="M86" s="8" t="s">
+      <c r="M86" s="6" t="s">
         <v>175</v>
       </c>
       <c r="N86" t="str">
         <f t="shared" si="5"/>
         <v>shadow creatures</v>
       </c>
-      <c r="O86" s="9" t="str">
+      <c r="O86" s="7" t="str">
         <f t="shared" si="6"/>
         <v>shadow_creatures</v>
       </c>
@@ -14691,7 +14698,7 @@
       </c>
     </row>
     <row r="87" spans="1:20">
-      <c r="A87" s="7"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="4" t="s">
         <v>176</v>
       </c>
@@ -14712,14 +14719,14 @@
         <v>53</v>
       </c>
       <c r="I87" s="4"/>
-      <c r="M87" s="8" t="s">
+      <c r="M87" s="6" t="s">
         <v>176</v>
       </c>
       <c r="N87" t="str">
         <f t="shared" si="5"/>
         <v>shatter</v>
       </c>
-      <c r="O87" s="9" t="str">
+      <c r="O87" s="7" t="str">
         <f t="shared" si="6"/>
         <v>shatter</v>
       </c>
@@ -14740,7 +14747,7 @@
       </c>
     </row>
     <row r="88" spans="1:20" ht="75" customHeight="1">
-      <c r="A88" s="7"/>
+      <c r="A88" s="15"/>
       <c r="B88" s="3" t="s">
         <v>177</v>
       </c>
@@ -14763,14 +14770,14 @@
         <v>41</v>
       </c>
       <c r="I88" s="4"/>
-      <c r="M88" s="8" t="s">
+      <c r="M88" s="6" t="s">
         <v>177</v>
       </c>
       <c r="N88" t="str">
         <f t="shared" si="5"/>
         <v>shock</v>
       </c>
-      <c r="O88" s="9" t="str">
+      <c r="O88" s="7" t="str">
         <f t="shared" si="6"/>
         <v>shock</v>
       </c>
@@ -14791,7 +14798,7 @@
       </c>
     </row>
     <row r="89" spans="1:20" ht="45">
-      <c r="A89" s="7"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="4" t="s">
         <v>178</v>
       </c>
@@ -14812,14 +14819,14 @@
         <v>56</v>
       </c>
       <c r="I89" s="4"/>
-      <c r="M89" s="8" t="s">
+      <c r="M89" s="6" t="s">
         <v>178</v>
       </c>
       <c r="N89" t="str">
         <f t="shared" si="5"/>
         <v>shroud of golubria</v>
       </c>
-      <c r="O89" s="9" t="str">
+      <c r="O89" s="7" t="str">
         <f t="shared" si="6"/>
         <v>shroud_of_golubria</v>
       </c>
@@ -14840,7 +14847,7 @@
       </c>
     </row>
     <row r="90" spans="1:20" ht="30" customHeight="1">
-      <c r="A90" s="7"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="4" t="s">
         <v>180</v>
       </c>
@@ -14861,14 +14868,14 @@
         <v>53</v>
       </c>
       <c r="I90" s="4"/>
-      <c r="M90" s="8" t="s">
+      <c r="M90" s="6" t="s">
         <v>180</v>
       </c>
       <c r="N90" t="str">
         <f t="shared" si="5"/>
         <v>silence</v>
       </c>
-      <c r="O90" s="9" t="str">
+      <c r="O90" s="7" t="str">
         <f t="shared" si="6"/>
         <v>silence</v>
       </c>
@@ -14889,7 +14896,7 @@
       </c>
     </row>
     <row r="91" spans="1:20" ht="30">
-      <c r="A91" s="7"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="4" t="s">
         <v>182</v>
       </c>
@@ -14908,14 +14915,14 @@
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="4"/>
-      <c r="M91" s="8" t="s">
+      <c r="M91" s="6" t="s">
         <v>182</v>
       </c>
       <c r="N91" t="str">
         <f t="shared" si="5"/>
         <v>simulacrum</v>
       </c>
-      <c r="O91" s="9" t="str">
+      <c r="O91" s="7" t="str">
         <f t="shared" si="6"/>
         <v>simulacrum</v>
       </c>
@@ -14936,7 +14943,7 @@
       </c>
     </row>
     <row r="92" spans="1:20" ht="15" customHeight="1">
-      <c r="A92" s="7"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="4" t="s">
         <v>184</v>
       </c>
@@ -14959,14 +14966,14 @@
         <v>159</v>
       </c>
       <c r="I92" s="4"/>
-      <c r="M92" s="8" t="s">
+      <c r="M92" s="6" t="s">
         <v>184</v>
       </c>
       <c r="N92" t="str">
         <f t="shared" si="5"/>
         <v>slow</v>
       </c>
-      <c r="O92" s="9" t="str">
+      <c r="O92" s="7" t="str">
         <f t="shared" si="6"/>
         <v>slow</v>
       </c>
@@ -14987,7 +14994,7 @@
       </c>
     </row>
     <row r="93" spans="1:20" ht="30">
-      <c r="A93" s="7"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="3" t="s">
         <v>185</v>
       </c>
@@ -15008,14 +15015,14 @@
         <v>25</v>
       </c>
       <c r="I93" s="4"/>
-      <c r="M93" s="8" t="s">
+      <c r="M93" s="6" t="s">
         <v>185</v>
       </c>
       <c r="N93" t="str">
         <f t="shared" si="5"/>
         <v>song of slaying</v>
       </c>
-      <c r="O93" s="9" t="str">
+      <c r="O93" s="7" t="str">
         <f t="shared" si="6"/>
         <v>song_of_slaying</v>
       </c>
@@ -15057,14 +15064,14 @@
         <v>188</v>
       </c>
       <c r="I94" s="4"/>
-      <c r="M94" s="8" t="s">
+      <c r="M94" s="6" t="s">
         <v>186</v>
       </c>
       <c r="N94" t="str">
         <f t="shared" si="5"/>
         <v>spectral weapon</v>
       </c>
-      <c r="O94" s="9" t="str">
+      <c r="O94" s="7" t="str">
         <f t="shared" si="6"/>
         <v>spectral_weapon</v>
       </c>
@@ -15104,14 +15111,14 @@
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="4"/>
-      <c r="M95" s="8" t="s">
+      <c r="M95" s="6" t="s">
         <v>189</v>
       </c>
       <c r="N95" t="str">
         <f t="shared" si="5"/>
         <v>spellforged servitor</v>
       </c>
-      <c r="O95" s="9" t="str">
+      <c r="O95" s="7" t="str">
         <f t="shared" si="6"/>
         <v>spellforged_servitor</v>
       </c>
@@ -15132,7 +15139,7 @@
       </c>
     </row>
     <row r="96" spans="1:20" ht="15" customHeight="1">
-      <c r="A96" s="7"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="3" t="s">
         <v>191</v>
       </c>
@@ -15153,14 +15160,14 @@
         <v>36</v>
       </c>
       <c r="I96" s="4"/>
-      <c r="M96" s="8" t="s">
+      <c r="M96" s="6" t="s">
         <v>191</v>
       </c>
       <c r="N96" t="str">
         <f t="shared" si="5"/>
         <v>spider form</v>
       </c>
-      <c r="O96" s="9" t="str">
+      <c r="O96" s="7" t="str">
         <f t="shared" si="6"/>
         <v>spider_form</v>
       </c>
@@ -15181,7 +15188,7 @@
       </c>
     </row>
     <row r="97" spans="1:20" ht="30">
-      <c r="A97" s="7"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="3" t="s">
         <v>192</v>
       </c>
@@ -15204,14 +15211,14 @@
         <v>53</v>
       </c>
       <c r="I97" s="4"/>
-      <c r="M97" s="8" t="s">
+      <c r="M97" s="6" t="s">
         <v>192</v>
       </c>
       <c r="N97" t="str">
         <f t="shared" si="5"/>
         <v>starburst</v>
       </c>
-      <c r="O97" s="9" t="str">
+      <c r="O97" s="7" t="str">
         <f t="shared" si="6"/>
         <v>starburst</v>
       </c>
@@ -15232,7 +15239,7 @@
       </c>
     </row>
     <row r="98" spans="1:20" ht="15" customHeight="1">
-      <c r="A98" s="7"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="4" t="s">
         <v>193</v>
       </c>
@@ -15255,14 +15262,14 @@
         <v>53</v>
       </c>
       <c r="I98" s="4"/>
-      <c r="M98" s="8" t="s">
+      <c r="M98" s="6" t="s">
         <v>193</v>
       </c>
       <c r="N98" t="str">
         <f t="shared" si="5"/>
         <v>static discharge</v>
       </c>
-      <c r="O98" s="9" t="str">
+      <c r="O98" s="7" t="str">
         <f t="shared" si="6"/>
         <v>static_discharge</v>
       </c>
@@ -15283,7 +15290,7 @@
       </c>
     </row>
     <row r="99" spans="1:20" ht="45">
-      <c r="A99" s="7"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="4" t="s">
         <v>194</v>
       </c>
@@ -15304,14 +15311,14 @@
         <v>36</v>
       </c>
       <c r="I99" s="4"/>
-      <c r="M99" s="8" t="s">
+      <c r="M99" s="6" t="s">
         <v>194</v>
       </c>
       <c r="N99" t="str">
         <f t="shared" si="5"/>
         <v>statue form</v>
       </c>
-      <c r="O99" s="9" t="str">
+      <c r="O99" s="7" t="str">
         <f t="shared" si="6"/>
         <v>statue_form</v>
       </c>
@@ -15353,14 +15360,14 @@
         <v>11</v>
       </c>
       <c r="I100" s="4"/>
-      <c r="M100" s="8" t="s">
+      <c r="M100" s="6" t="s">
         <v>195</v>
       </c>
       <c r="N100" t="str">
         <f t="shared" si="5"/>
         <v>sticks to snakes</v>
       </c>
-      <c r="O100" s="9" t="str">
+      <c r="O100" s="7" t="str">
         <f t="shared" si="6"/>
         <v>sticks_to_snakes</v>
       </c>
@@ -15381,7 +15388,7 @@
       </c>
     </row>
     <row r="101" spans="1:20" ht="15" customHeight="1">
-      <c r="A101" s="7"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="3" t="s">
         <v>196</v>
       </c>
@@ -15404,14 +15411,14 @@
         <v>41</v>
       </c>
       <c r="I101" s="4"/>
-      <c r="M101" s="8" t="s">
+      <c r="M101" s="6" t="s">
         <v>196</v>
       </c>
       <c r="N101" t="str">
         <f t="shared" si="5"/>
         <v>sticky flame</v>
       </c>
-      <c r="O101" s="9" t="str">
+      <c r="O101" s="7" t="str">
         <f t="shared" si="6"/>
         <v>sticky_flame</v>
       </c>
@@ -15432,7 +15439,7 @@
       </c>
     </row>
     <row r="102" spans="1:20" ht="60">
-      <c r="A102" s="7"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="3" t="s">
         <v>197</v>
       </c>
@@ -15455,14 +15462,14 @@
         <v>41</v>
       </c>
       <c r="I102" s="4"/>
-      <c r="M102" s="8" t="s">
+      <c r="M102" s="6" t="s">
         <v>197</v>
       </c>
       <c r="N102" t="str">
         <f t="shared" si="5"/>
         <v>sting</v>
       </c>
-      <c r="O102" s="9" t="str">
+      <c r="O102" s="7" t="str">
         <f t="shared" si="6"/>
         <v>sting</v>
       </c>
@@ -15483,7 +15490,7 @@
       </c>
     </row>
     <row r="103" spans="1:20" ht="15" customHeight="1">
-      <c r="A103" s="7"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="4" t="s">
         <v>198</v>
       </c>
@@ -15506,14 +15513,14 @@
         <v>41</v>
       </c>
       <c r="I103" s="4"/>
-      <c r="M103" s="8" t="s">
+      <c r="M103" s="6" t="s">
         <v>198</v>
       </c>
       <c r="N103" t="str">
         <f t="shared" si="5"/>
         <v>stone arrow</v>
       </c>
-      <c r="O103" s="9" t="str">
+      <c r="O103" s="7" t="str">
         <f t="shared" si="6"/>
         <v>stone_arrow</v>
       </c>
@@ -15534,7 +15541,7 @@
       </c>
     </row>
     <row r="104" spans="1:20" ht="45">
-      <c r="A104" s="7"/>
+      <c r="A104" s="15"/>
       <c r="B104" s="4" t="s">
         <v>199</v>
       </c>
@@ -15555,14 +15562,14 @@
         <v>25</v>
       </c>
       <c r="I104" s="4"/>
-      <c r="M104" s="8" t="s">
+      <c r="M104" s="6" t="s">
         <v>199</v>
       </c>
       <c r="N104" t="str">
         <f t="shared" si="5"/>
         <v>sublimation of blood</v>
       </c>
-      <c r="O104" s="9" t="str">
+      <c r="O104" s="7" t="str">
         <f t="shared" si="6"/>
         <v>sublimation_of_blood</v>
       </c>
@@ -15583,7 +15590,7 @@
       </c>
     </row>
     <row r="105" spans="1:20" ht="15" customHeight="1">
-      <c r="A105" s="7"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="3" t="s">
         <v>200</v>
       </c>
@@ -15604,14 +15611,14 @@
         <v>201</v>
       </c>
       <c r="I105" s="4"/>
-      <c r="M105" s="8" t="s">
+      <c r="M105" s="6" t="s">
         <v>200</v>
       </c>
       <c r="N105" t="str">
         <f t="shared" si="5"/>
         <v>summon demon</v>
       </c>
-      <c r="O105" s="9" t="str">
+      <c r="O105" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_demon</v>
       </c>
@@ -15632,7 +15639,7 @@
       </c>
     </row>
     <row r="106" spans="1:20" ht="45">
-      <c r="A106" s="7"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="4" t="s">
         <v>202</v>
       </c>
@@ -15651,14 +15658,14 @@
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="4"/>
-      <c r="M106" s="8" t="s">
+      <c r="M106" s="6" t="s">
         <v>202</v>
       </c>
       <c r="N106" t="str">
         <f t="shared" si="5"/>
         <v>summon forest</v>
       </c>
-      <c r="O106" s="9" t="str">
+      <c r="O106" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_forest</v>
       </c>
@@ -15700,14 +15707,14 @@
         <v>201</v>
       </c>
       <c r="I107" s="4"/>
-      <c r="M107" s="8" t="s">
+      <c r="M107" s="6" t="s">
         <v>203</v>
       </c>
       <c r="N107" t="str">
         <f t="shared" si="5"/>
         <v>summon greater demon</v>
       </c>
-      <c r="O107" s="9" t="str">
+      <c r="O107" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_greater_demon</v>
       </c>
@@ -15728,7 +15735,7 @@
       </c>
     </row>
     <row r="108" spans="1:20" ht="15" customHeight="1">
-      <c r="A108" s="7"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="3" t="s">
         <v>204</v>
       </c>
@@ -15747,14 +15754,14 @@
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="4"/>
-      <c r="M108" s="8" t="s">
+      <c r="M108" s="6" t="s">
         <v>204</v>
       </c>
       <c r="N108" t="str">
         <f t="shared" si="5"/>
         <v>summon guardian golem</v>
       </c>
-      <c r="O108" s="9" t="str">
+      <c r="O108" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_guardian_golem</v>
       </c>
@@ -15775,7 +15782,7 @@
       </c>
     </row>
     <row r="109" spans="1:20" ht="75">
-      <c r="A109" s="7"/>
+      <c r="A109" s="15"/>
       <c r="B109" s="3" t="s">
         <v>206</v>
       </c>
@@ -15796,14 +15803,14 @@
         <v>207</v>
       </c>
       <c r="I109" s="4"/>
-      <c r="M109" s="8" t="s">
+      <c r="M109" s="6" t="s">
         <v>206</v>
       </c>
       <c r="N109" t="str">
         <f t="shared" si="5"/>
         <v>summon horrible things</v>
       </c>
-      <c r="O109" s="9" t="str">
+      <c r="O109" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_horrible_things</v>
       </c>
@@ -15824,7 +15831,7 @@
       </c>
     </row>
     <row r="110" spans="1:20" ht="30">
-      <c r="A110" s="7"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="4" t="s">
         <v>208</v>
       </c>
@@ -15845,14 +15852,14 @@
         <v>149</v>
       </c>
       <c r="I110" s="4"/>
-      <c r="M110" s="8" t="s">
+      <c r="M110" s="6" t="s">
         <v>208</v>
       </c>
       <c r="N110" t="str">
         <f t="shared" si="5"/>
         <v>summon hydra</v>
       </c>
-      <c r="O110" s="9" t="str">
+      <c r="O110" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_hydra</v>
       </c>
@@ -15873,7 +15880,7 @@
       </c>
     </row>
     <row r="111" spans="1:20" ht="15" customHeight="1">
-      <c r="A111" s="7"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="4" t="s">
         <v>209</v>
       </c>
@@ -15892,14 +15899,14 @@
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="4"/>
-      <c r="M111" s="8" t="s">
+      <c r="M111" s="6" t="s">
         <v>209</v>
       </c>
       <c r="N111" t="str">
         <f t="shared" si="5"/>
         <v>summon ice beast</v>
       </c>
-      <c r="O111" s="9" t="str">
+      <c r="O111" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_ice_beast</v>
       </c>
@@ -15920,7 +15927,7 @@
       </c>
     </row>
     <row r="112" spans="1:20" ht="45">
-      <c r="A112" s="7"/>
+      <c r="A112" s="15"/>
       <c r="B112" s="4" t="s">
         <v>211</v>
       </c>
@@ -15941,14 +15948,14 @@
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="4"/>
-      <c r="M112" s="8" t="s">
+      <c r="M112" s="6" t="s">
         <v>211</v>
       </c>
       <c r="N112" t="str">
         <f t="shared" si="5"/>
         <v>summon lightning spire</v>
       </c>
-      <c r="O112" s="9" t="str">
+      <c r="O112" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_lightning_spire</v>
       </c>
@@ -15990,14 +15997,14 @@
         <v>149</v>
       </c>
       <c r="I113" s="4"/>
-      <c r="M113" s="8" t="s">
+      <c r="M113" s="6" t="s">
         <v>213</v>
       </c>
       <c r="N113" t="str">
         <f t="shared" si="5"/>
         <v>summon mana viper</v>
       </c>
-      <c r="O113" s="9" t="str">
+      <c r="O113" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_mana_viper</v>
       </c>
@@ -16037,14 +16044,14 @@
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="4"/>
-      <c r="M114" s="8" t="s">
+      <c r="M114" s="6" t="s">
         <v>214</v>
       </c>
       <c r="N114" t="str">
         <f t="shared" si="5"/>
         <v>summon small mammal</v>
       </c>
-      <c r="O114" s="9" t="str">
+      <c r="O114" s="7" t="str">
         <f t="shared" si="6"/>
         <v>summon_small_mammal</v>
       </c>
@@ -16086,14 +16093,14 @@
         <v>217</v>
       </c>
       <c r="I115" s="4"/>
-      <c r="M115" s="8" t="s">
+      <c r="M115" s="6" t="s">
         <v>215</v>
       </c>
       <c r="N115" t="str">
         <f t="shared" si="5"/>
         <v>swiftness</v>
       </c>
-      <c r="O115" s="9" t="str">
+      <c r="O115" s="7" t="str">
         <f t="shared" si="6"/>
         <v>swiftness</v>
       </c>
@@ -16137,14 +16144,14 @@
         <v>219</v>
       </c>
       <c r="I116" s="4"/>
-      <c r="M116" s="8" t="s">
+      <c r="M116" s="6" t="s">
         <v>218</v>
       </c>
       <c r="N116" t="str">
         <f t="shared" si="5"/>
         <v>teleport other</v>
       </c>
-      <c r="O116" s="9" t="str">
+      <c r="O116" s="7" t="str">
         <f t="shared" si="6"/>
         <v>teleport_other</v>
       </c>
@@ -16165,7 +16172,7 @@
       </c>
     </row>
     <row r="117" spans="1:20" ht="15" customHeight="1">
-      <c r="A117" s="7"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="4" t="s">
         <v>220</v>
       </c>
@@ -16188,14 +16195,14 @@
         <v>53</v>
       </c>
       <c r="I117" s="4"/>
-      <c r="M117" s="8" t="s">
+      <c r="M117" s="6" t="s">
         <v>220</v>
       </c>
       <c r="N117" t="str">
         <f t="shared" si="5"/>
         <v>tornado</v>
       </c>
-      <c r="O117" s="9" t="str">
+      <c r="O117" s="7" t="str">
         <f t="shared" si="6"/>
         <v>tornado</v>
       </c>
@@ -16216,7 +16223,7 @@
       </c>
     </row>
     <row r="118" spans="1:20" ht="105">
-      <c r="A118" s="7"/>
+      <c r="A118" s="15"/>
       <c r="B118" s="4" t="s">
         <v>221</v>
       </c>
@@ -16239,14 +16246,14 @@
         <v>14</v>
       </c>
       <c r="I118" s="4"/>
-      <c r="M118" s="8" t="s">
+      <c r="M118" s="6" t="s">
         <v>221</v>
       </c>
       <c r="N118" t="str">
         <f t="shared" si="5"/>
         <v>tukima's dance</v>
       </c>
-      <c r="O118" s="9" t="str">
+      <c r="O118" s="7" t="str">
         <f t="shared" si="6"/>
         <v>tukima's_dance</v>
       </c>
@@ -16290,14 +16297,14 @@
         <v>223</v>
       </c>
       <c r="I119" s="4"/>
-      <c r="M119" s="8" t="s">
+      <c r="M119" s="6" t="s">
         <v>222</v>
       </c>
       <c r="N119" t="str">
         <f t="shared" si="5"/>
         <v>vampiric draining</v>
       </c>
-      <c r="O119" s="9" t="str">
+      <c r="O119" s="7" t="str">
         <f t="shared" si="6"/>
         <v>vampiric_draining</v>
       </c>
@@ -16338,14 +16345,14 @@
         <v>226</v>
       </c>
       <c r="I120" s="4"/>
-      <c r="M120" s="8" t="s">
+      <c r="M120" s="6" t="s">
         <v>224</v>
       </c>
       <c r="N120" t="str">
         <f t="shared" si="5"/>
         <v>yara's violent unravelling</v>
       </c>
-      <c r="O120" s="9" t="str">
+      <c r="O120" s="7" t="str">
         <f t="shared" si="6"/>
         <v>yara's_violent_unravelling</v>
       </c>
@@ -16363,7 +16370,7 @@
       </c>
     </row>
     <row r="121" spans="1:20" ht="15" customHeight="1">
-      <c r="A121" s="7"/>
+      <c r="A121" s="15"/>
       <c r="B121" s="4"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -16375,72 +16382,72 @@
       <c r="M121" s="4"/>
     </row>
     <row r="122" spans="1:20">
-      <c r="A122" s="7"/>
+      <c r="A122" s="15"/>
       <c r="I122" s="4"/>
       <c r="M122" s="4"/>
     </row>
     <row r="123" spans="1:20" ht="15" customHeight="1">
-      <c r="A123" s="7"/>
+      <c r="A123" s="15"/>
       <c r="I123" s="4"/>
       <c r="M123" s="4"/>
     </row>
     <row r="124" spans="1:20">
-      <c r="A124" s="7"/>
+      <c r="A124" s="15"/>
       <c r="I124" s="4"/>
       <c r="M124" s="4"/>
     </row>
     <row r="125" spans="1:20" ht="15" customHeight="1">
-      <c r="A125" s="7"/>
+      <c r="A125" s="15"/>
       <c r="I125" s="4"/>
       <c r="M125" s="4"/>
     </row>
     <row r="126" spans="1:20">
-      <c r="A126" s="7"/>
+      <c r="A126" s="15"/>
       <c r="I126" s="4"/>
       <c r="M126" s="4"/>
     </row>
     <row r="127" spans="1:20">
-      <c r="A127" s="7"/>
+      <c r="A127" s="15"/>
       <c r="I127" s="4"/>
       <c r="M127" s="4"/>
     </row>
     <row r="128" spans="1:20" ht="15" customHeight="1">
-      <c r="A128" s="7"/>
+      <c r="A128" s="15"/>
       <c r="I128" s="4"/>
       <c r="M128" s="4"/>
     </row>
     <row r="129" spans="1:13">
-      <c r="A129" s="7"/>
+      <c r="A129" s="15"/>
       <c r="I129" s="4"/>
       <c r="M129" s="4"/>
     </row>
     <row r="130" spans="1:13" ht="15" customHeight="1">
-      <c r="A130" s="7"/>
+      <c r="A130" s="15"/>
       <c r="I130" s="4"/>
       <c r="M130" s="4"/>
     </row>
     <row r="131" spans="1:13">
-      <c r="A131" s="7"/>
+      <c r="A131" s="15"/>
       <c r="I131" s="4"/>
       <c r="M131" s="4"/>
     </row>
     <row r="132" spans="1:13" ht="15" customHeight="1">
-      <c r="A132" s="7"/>
+      <c r="A132" s="15"/>
       <c r="I132" s="4"/>
       <c r="M132" s="4"/>
     </row>
     <row r="133" spans="1:13">
-      <c r="A133" s="7"/>
+      <c r="A133" s="15"/>
       <c r="I133" s="4"/>
       <c r="M133" s="4"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
-      <c r="A134" s="7"/>
+      <c r="A134" s="15"/>
       <c r="I134" s="4"/>
       <c r="M134" s="4"/>
     </row>
     <row r="135" spans="1:13">
-      <c r="A135" s="7"/>
+      <c r="A135" s="15"/>
       <c r="I135" s="4"/>
       <c r="M135" s="4"/>
     </row>
@@ -16455,22 +16462,22 @@
       <c r="M137" s="4"/>
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1">
-      <c r="A138" s="7"/>
+      <c r="A138" s="15"/>
       <c r="I138" s="4"/>
       <c r="M138" s="4"/>
     </row>
     <row r="139" spans="1:13">
-      <c r="A139" s="7"/>
+      <c r="A139" s="15"/>
       <c r="I139" s="4"/>
       <c r="M139" s="4"/>
     </row>
     <row r="140" spans="1:13">
-      <c r="A140" s="7"/>
+      <c r="A140" s="15"/>
       <c r="I140" s="4"/>
       <c r="M140" s="4"/>
     </row>
     <row r="141" spans="1:13">
-      <c r="A141" s="7"/>
+      <c r="A141" s="15"/>
       <c r="I141" s="4"/>
       <c r="M141" s="4"/>
     </row>
@@ -16480,47 +16487,47 @@
       <c r="M142" s="4"/>
     </row>
     <row r="143" spans="1:13" ht="15" customHeight="1">
-      <c r="A143" s="7"/>
+      <c r="A143" s="15"/>
       <c r="I143" s="4"/>
       <c r="M143" s="4"/>
     </row>
     <row r="144" spans="1:13">
-      <c r="A144" s="7"/>
+      <c r="A144" s="15"/>
       <c r="I144" s="4"/>
       <c r="M144" s="4"/>
     </row>
     <row r="145" spans="1:13" ht="15" customHeight="1">
-      <c r="A145" s="7"/>
+      <c r="A145" s="15"/>
       <c r="I145" s="4"/>
       <c r="M145" s="4"/>
     </row>
     <row r="146" spans="1:13">
-      <c r="A146" s="7"/>
+      <c r="A146" s="15"/>
       <c r="I146" s="4"/>
       <c r="M146" s="4"/>
     </row>
     <row r="147" spans="1:13">
-      <c r="A147" s="7"/>
+      <c r="A147" s="15"/>
       <c r="I147" s="4"/>
       <c r="M147" s="4"/>
     </row>
     <row r="148" spans="1:13" ht="15" customHeight="1">
-      <c r="A148" s="7"/>
+      <c r="A148" s="15"/>
       <c r="I148" s="4"/>
       <c r="M148" s="4"/>
     </row>
     <row r="149" spans="1:13">
-      <c r="A149" s="7"/>
+      <c r="A149" s="15"/>
       <c r="I149" s="4"/>
       <c r="M149" s="4"/>
     </row>
     <row r="150" spans="1:13" ht="45" customHeight="1">
-      <c r="A150" s="7"/>
+      <c r="A150" s="15"/>
       <c r="I150" s="4"/>
       <c r="M150" s="4"/>
     </row>
     <row r="151" spans="1:13">
-      <c r="A151" s="7"/>
+      <c r="A151" s="15"/>
       <c r="I151" s="4"/>
       <c r="M151" s="4"/>
     </row>
@@ -16550,22 +16557,22 @@
       <c r="M156" s="4"/>
     </row>
     <row r="157" spans="1:13" ht="15" customHeight="1">
-      <c r="A157" s="7"/>
+      <c r="A157" s="15"/>
       <c r="I157" s="4"/>
       <c r="M157" s="4"/>
     </row>
     <row r="158" spans="1:13">
-      <c r="A158" s="7"/>
+      <c r="A158" s="15"/>
       <c r="I158" s="4"/>
       <c r="M158" s="4"/>
     </row>
     <row r="159" spans="1:13" ht="15" customHeight="1">
-      <c r="A159" s="7"/>
+      <c r="A159" s="15"/>
       <c r="I159" s="4"/>
       <c r="M159" s="4"/>
     </row>
     <row r="160" spans="1:13">
-      <c r="A160" s="7"/>
+      <c r="A160" s="15"/>
       <c r="I160" s="4"/>
       <c r="M160" s="4"/>
     </row>
@@ -16585,22 +16592,22 @@
       <c r="M163" s="4"/>
     </row>
     <row r="164" spans="1:13" ht="15" customHeight="1">
-      <c r="A164" s="7"/>
+      <c r="A164" s="15"/>
       <c r="I164" s="4"/>
       <c r="M164" s="4"/>
     </row>
     <row r="165" spans="1:13">
-      <c r="A165" s="7"/>
+      <c r="A165" s="15"/>
       <c r="I165" s="4"/>
       <c r="M165" s="4"/>
     </row>
     <row r="166" spans="1:13" ht="15" customHeight="1">
-      <c r="A166" s="7"/>
+      <c r="A166" s="15"/>
       <c r="I166" s="4"/>
       <c r="M166" s="4"/>
     </row>
     <row r="167" spans="1:13">
-      <c r="A167" s="7"/>
+      <c r="A167" s="15"/>
       <c r="I167" s="4"/>
       <c r="M167" s="4"/>
     </row>
@@ -16610,12 +16617,12 @@
       <c r="M168" s="4"/>
     </row>
     <row r="169" spans="1:13" ht="15" customHeight="1">
-      <c r="A169" s="7"/>
+      <c r="A169" s="15"/>
       <c r="I169" s="4"/>
       <c r="M169" s="4"/>
     </row>
     <row r="170" spans="1:13">
-      <c r="A170" s="7"/>
+      <c r="A170" s="15"/>
       <c r="I170" s="4"/>
       <c r="M170" s="4"/>
     </row>
@@ -16635,67 +16642,67 @@
       <c r="M173" s="4"/>
     </row>
     <row r="174" spans="1:13" ht="15" customHeight="1">
-      <c r="A174" s="7"/>
+      <c r="A174" s="15"/>
       <c r="I174" s="4"/>
       <c r="M174" s="4"/>
     </row>
     <row r="175" spans="1:13">
-      <c r="A175" s="7"/>
+      <c r="A175" s="15"/>
       <c r="I175" s="4"/>
       <c r="M175" s="4"/>
     </row>
     <row r="176" spans="1:13" ht="15" customHeight="1">
-      <c r="A176" s="7"/>
+      <c r="A176" s="15"/>
       <c r="I176" s="4"/>
       <c r="M176" s="4"/>
     </row>
     <row r="177" spans="1:13">
-      <c r="A177" s="7"/>
+      <c r="A177" s="15"/>
       <c r="I177" s="4"/>
       <c r="M177" s="4"/>
     </row>
     <row r="178" spans="1:13">
-      <c r="A178" s="7"/>
+      <c r="A178" s="15"/>
       <c r="I178" s="4"/>
       <c r="M178" s="4"/>
     </row>
     <row r="179" spans="1:13" ht="15" customHeight="1">
-      <c r="A179" s="7"/>
+      <c r="A179" s="15"/>
       <c r="I179" s="4"/>
       <c r="M179" s="4"/>
     </row>
     <row r="180" spans="1:13">
-      <c r="A180" s="7"/>
+      <c r="A180" s="15"/>
       <c r="I180" s="4"/>
       <c r="M180" s="4"/>
     </row>
     <row r="181" spans="1:13" ht="15" customHeight="1">
-      <c r="A181" s="7"/>
+      <c r="A181" s="15"/>
       <c r="I181" s="4"/>
       <c r="M181" s="4"/>
     </row>
     <row r="182" spans="1:13">
-      <c r="A182" s="7"/>
+      <c r="A182" s="15"/>
       <c r="I182" s="4"/>
       <c r="M182" s="4"/>
     </row>
     <row r="183" spans="1:13" ht="15" customHeight="1">
-      <c r="A183" s="7"/>
+      <c r="A183" s="15"/>
       <c r="I183" s="4"/>
       <c r="M183" s="4"/>
     </row>
     <row r="184" spans="1:13">
-      <c r="A184" s="7"/>
+      <c r="A184" s="15"/>
       <c r="I184" s="4"/>
       <c r="M184" s="4"/>
     </row>
     <row r="185" spans="1:13" ht="15" customHeight="1">
-      <c r="A185" s="7"/>
+      <c r="A185" s="15"/>
       <c r="I185" s="4"/>
       <c r="M185" s="4"/>
     </row>
     <row r="186" spans="1:13">
-      <c r="A186" s="7"/>
+      <c r="A186" s="15"/>
       <c r="I186" s="4"/>
       <c r="M186" s="4"/>
     </row>
@@ -16705,22 +16712,22 @@
       <c r="M187" s="4"/>
     </row>
     <row r="188" spans="1:13" ht="15" customHeight="1">
-      <c r="A188" s="7"/>
+      <c r="A188" s="15"/>
       <c r="I188" s="4"/>
       <c r="M188" s="4"/>
     </row>
     <row r="189" spans="1:13">
-      <c r="A189" s="7"/>
+      <c r="A189" s="15"/>
       <c r="I189" s="4"/>
       <c r="M189" s="4"/>
     </row>
     <row r="190" spans="1:13" ht="60" customHeight="1">
-      <c r="A190" s="7"/>
+      <c r="A190" s="15"/>
       <c r="I190" s="4"/>
       <c r="M190" s="4"/>
     </row>
     <row r="191" spans="1:13">
-      <c r="A191" s="7"/>
+      <c r="A191" s="15"/>
       <c r="I191" s="4"/>
       <c r="M191" s="4"/>
     </row>
@@ -16730,12 +16737,12 @@
       <c r="M192" s="4"/>
     </row>
     <row r="193" spans="1:13" ht="45" customHeight="1">
-      <c r="A193" s="7"/>
+      <c r="A193" s="15"/>
       <c r="I193" s="4"/>
       <c r="M193" s="4"/>
     </row>
     <row r="194" spans="1:13">
-      <c r="A194" s="7"/>
+      <c r="A194" s="15"/>
       <c r="I194" s="4"/>
       <c r="M194" s="4"/>
     </row>
@@ -16744,6 +16751,58 @@
     <sortCondition ref="T1:T232"/>
   </sortState>
   <mergeCells count="68">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="A138:A139"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="A193:A194"/>
     <mergeCell ref="A190:A191"/>
@@ -16760,58 +16819,6 @@
     <mergeCell ref="A159:A160"/>
     <mergeCell ref="A157:A158"/>
     <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" tooltip="Absolute Zero" display="http://crawl.chaosforge.org/Absolute_Zero" xr:uid="{0B7D80AD-41C3-4378-86E9-351B477A2B9F}"/>
@@ -17015,51 +17022,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>349</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>536</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>566</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>355</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>359</v>
       </c>
       <c r="H2" t="str">
@@ -17075,22 +17082,22 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="30">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>361</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>363</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>365</v>
       </c>
       <c r="H3" t="str">
@@ -17106,22 +17113,22 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="30">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="11" t="s">
         <v>368</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="11" t="s">
         <v>369</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="11" t="s">
         <v>370</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="11" t="s">
         <v>371</v>
       </c>
       <c r="H4" t="str">
@@ -17137,22 +17144,22 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="30">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>374</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>376</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>377</v>
       </c>
       <c r="H5" t="str">
@@ -17168,22 +17175,22 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="30">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>379</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>381</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="11" t="s">
         <v>382</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="11" t="s">
         <v>383</v>
       </c>
       <c r="H6" t="str">
@@ -17199,22 +17206,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>385</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>386</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>387</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>388</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>389</v>
       </c>
       <c r="H7" t="str">
@@ -17230,22 +17237,22 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="30">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>391</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>393</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>394</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="11" t="s">
         <v>395</v>
       </c>
       <c r="H8" t="str">
@@ -17261,22 +17268,22 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="90">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>397</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>401</v>
       </c>
       <c r="H9" t="str">
@@ -17292,22 +17299,22 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>403</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>404</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>405</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="11" t="s">
         <v>406</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="11" t="s">
         <v>407</v>
       </c>
       <c r="H10" t="str">
@@ -17323,22 +17330,22 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>411</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="11" t="s">
         <v>412</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>413</v>
       </c>
       <c r="H11" t="str">
@@ -17354,22 +17361,22 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>415</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>416</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="11" t="s">
         <v>418</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="11" t="s">
         <v>419</v>
       </c>
       <c r="H12" t="str">
@@ -17385,22 +17392,22 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="11" t="s">
         <v>421</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="11" t="s">
         <v>425</v>
       </c>
       <c r="H13" t="str">
@@ -17416,22 +17423,22 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>427</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>428</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>429</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>430</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>431</v>
       </c>
       <c r="H14" t="str">
@@ -17447,22 +17454,22 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="30">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>433</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>434</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="11" t="s">
         <v>435</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="11" t="s">
         <v>436</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>437</v>
       </c>
       <c r="H15" t="str">
@@ -17478,22 +17485,22 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="45">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>439</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>440</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>441</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>442</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>443</v>
       </c>
       <c r="H16" t="str">
@@ -17509,22 +17516,22 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="30">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>445</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>446</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>447</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="11" t="s">
         <v>448</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>449</v>
       </c>
       <c r="H17" t="str">
@@ -17540,22 +17547,22 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>451</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>452</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="11" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>455</v>
       </c>
       <c r="H18" t="str">
@@ -17571,22 +17578,22 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>456</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>457</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>458</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="11" t="s">
         <v>459</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="11" t="s">
         <v>460</v>
       </c>
       <c r="H19" t="str">
@@ -17602,22 +17609,22 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>461</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>462</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>463</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
         <v>464</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="11" t="s">
         <v>465</v>
       </c>
       <c r="H20" t="str">
@@ -17633,22 +17640,22 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="60">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>466</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="11" t="s">
         <v>467</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>468</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>469</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="11" t="s">
         <v>470</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="11" t="s">
         <v>471</v>
       </c>
       <c r="H21" t="str">
@@ -17664,22 +17671,22 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="30">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>472</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>473</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>474</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="11" t="s">
         <v>475</v>
       </c>
-      <c r="F22" s="13" t="s">
+      <c r="F22" s="11" t="s">
         <v>476</v>
       </c>
       <c r="H22" t="str">
@@ -17695,22 +17702,22 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="45">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="6" t="s">
         <v>477</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="11" t="s">
         <v>478</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>479</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>480</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="11" t="s">
         <v>482</v>
       </c>
       <c r="H23" t="str">
@@ -17726,22 +17733,22 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>483</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>484</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="11" t="s">
         <v>486</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="11" t="s">
         <v>487</v>
       </c>
       <c r="H24" t="str">
@@ -17757,22 +17764,22 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="6" t="s">
         <v>488</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>490</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="11" t="s">
         <v>492</v>
       </c>
-      <c r="F25" s="13" t="s">
+      <c r="F25" s="11" t="s">
         <v>493</v>
       </c>
       <c r="H25" t="str">
@@ -17788,22 +17795,22 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="30">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>495</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>496</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="11" t="s">
         <v>497</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="11" t="s">
         <v>498</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="11" t="s">
         <v>499</v>
       </c>
       <c r="H26" t="str">
@@ -17819,22 +17826,22 @@
       </c>
     </row>
     <row r="27" spans="1:10" ht="30">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>500</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>501</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>502</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="11" t="s">
         <v>504</v>
       </c>
-      <c r="F27" s="13" t="s">
+      <c r="F27" s="11" t="s">
         <v>505</v>
       </c>
       <c r="H27" t="str">
@@ -17850,22 +17857,22 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="30">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="6" t="s">
         <v>506</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>507</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="11" t="s">
         <v>509</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="11" t="s">
         <v>510</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="11" t="s">
         <v>511</v>
       </c>
       <c r="H28" t="str">
@@ -17881,22 +17888,22 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="6" t="s">
         <v>512</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="11" t="s">
         <v>513</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="11" t="s">
         <v>514</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="11" t="s">
         <v>515</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="11" t="s">
         <v>516</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="11" t="s">
         <v>517</v>
       </c>
       <c r="H29" t="str">
@@ -17912,22 +17919,22 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="30">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="6" t="s">
         <v>518</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="11" t="s">
         <v>519</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="11" t="s">
         <v>521</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="11" t="s">
         <v>522</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="11" t="s">
         <v>523</v>
       </c>
       <c r="H30" t="str">
@@ -17943,22 +17950,22 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="11" t="s">
         <v>525</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>526</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="11" t="s">
         <v>527</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="11" t="s">
         <v>528</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="11" t="s">
         <v>529</v>
       </c>
       <c r="H31" t="str">
@@ -17974,22 +17981,22 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="30">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="6" t="s">
         <v>530</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="11" t="s">
         <v>531</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>532</v>
       </c>
-      <c r="D32" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>533</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="11" t="s">
         <v>534</v>
       </c>
-      <c r="F32" s="13" t="s">
+      <c r="F32" s="11" t="s">
         <v>535</v>
       </c>
       <c r="H32" t="str">
@@ -18010,10 +18017,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{205C405B-3362-426C-A883-8DA14F508A14}">
+  <dimension ref="F12:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="12" spans="6:10">
+      <c r="J12" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="13" spans="6:10">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="6:10">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>828</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="6:10">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E9C651-19A5-494D-8095-C1365B59BB3C}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView topLeftCell="B64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
@@ -19876,12 +19936,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC10D0C3-A69E-4E6B-AEE8-F482A6FE85F2}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19920,7 +19980,7 @@
         <v>801</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D19" si="1">CONCATENATE("(", C2, " ", TRIM(SUBSTITUTE(B2, "pot", "")), ")")</f>
+        <f t="shared" ref="D2:D18" si="1">CONCATENATE("(", C2, " ", TRIM(SUBSTITUTE(B2, "pot", "")), ")")</f>
         <v>(potion berserkrage)</v>
       </c>
     </row>
@@ -20495,12 +20555,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9578DB-FD8E-4002-8B1E-A666019A80A1}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20511,7 +20571,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>803</v>
       </c>
       <c r="B1" t="str">
@@ -20524,7 +20584,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>804</v>
       </c>
       <c r="B2" t="str">
@@ -20537,7 +20597,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>805</v>
       </c>
       <c r="B3" t="str">
@@ -20550,7 +20610,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="6" t="s">
         <v>806</v>
       </c>
       <c r="B4" t="str">
@@ -20563,7 +20623,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>807</v>
       </c>
       <c r="B5" t="str">
@@ -20576,7 +20636,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>808</v>
       </c>
       <c r="B6" t="str">
@@ -20589,7 +20649,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>809</v>
       </c>
       <c r="B7" t="str">
@@ -20602,7 +20662,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>810</v>
       </c>
       <c r="B8" t="str">
@@ -20615,7 +20675,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="13" t="s">
         <v>811</v>
       </c>
       <c r="B9" t="str">
@@ -20628,7 +20688,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="13" t="s">
         <v>812</v>
       </c>
       <c r="B10" t="str">
@@ -20641,7 +20701,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="13" t="s">
         <v>813</v>
       </c>
       <c r="B11" t="str">
@@ -20654,7 +20714,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="6" t="s">
         <v>814</v>
       </c>
       <c r="B12" t="str">
@@ -20667,7 +20727,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="13" t="s">
         <v>815</v>
       </c>
       <c r="B13" t="str">
@@ -20680,7 +20740,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="6" t="s">
         <v>816</v>
       </c>
       <c r="B14" t="str">
@@ -20693,7 +20753,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="6" t="s">
         <v>817</v>
       </c>
       <c r="B15" t="str">
@@ -20706,7 +20766,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="6" t="s">
         <v>818</v>
       </c>
       <c r="B16" t="str">
@@ -20719,7 +20779,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="13" t="s">
         <v>819</v>
       </c>
       <c r="B17" t="str">
@@ -20732,7 +20792,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="13" t="s">
         <v>820</v>
       </c>
       <c r="B18" t="str">
@@ -20745,7 +20805,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="6" t="s">
         <v>821</v>
       </c>
       <c r="B19" t="str">
@@ -20758,7 +20818,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="6" t="s">
         <v>822</v>
       </c>
       <c r="B20" t="str">
@@ -20771,7 +20831,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>823</v>
       </c>
       <c r="B21" t="str">
@@ -20784,7 +20844,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="13" t="s">
         <v>824</v>
       </c>
       <c r="B22" t="str">
@@ -20797,7 +20857,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>825</v>
       </c>
       <c r="B23" t="str">
@@ -20810,7 +20870,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="6" t="s">
         <v>826</v>
       </c>
       <c r="B24" t="str">
@@ -20823,7 +20883,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="6" t="s">
         <v>827</v>
       </c>
       <c r="B25" t="str">

</xml_diff>

<commit_message>
updated pypi and documentation
</commit_message>
<xml_diff>
--- a/models/wiki_data_manually_entered.xlsx
+++ b/models/wiki_data_manually_entered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbe28fe5e73b7d58/Code Projects/dcss-ai-wrapper/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D82510D-BF94-4BF3-9B38-6F9BC717C70A}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E74E18A-B48C-4FE2-BBB2-AFB0697115CB}"/>
   <bookViews>
-    <workbookView xWindow="18705" yWindow="3735" windowWidth="31455" windowHeight="15435" activeTab="1" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
+    <workbookView xWindow="18360" yWindow="3390" windowWidth="28170" windowHeight="15435" activeTab="3" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="spells" sheetId="1" r:id="rId1"/>
@@ -2791,11 +2791,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10452,7 +10452,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -10476,8 +10476,8 @@
       <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="I1" s="14"/>
+      <c r="M1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T1" t="s">
@@ -10485,7 +10485,7 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="15"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -10495,8 +10495,8 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="15"/>
-      <c r="M2" s="15"/>
+      <c r="I2" s="14"/>
+      <c r="M2" s="14"/>
       <c r="P2" s="8" t="s">
         <v>227</v>
       </c>
@@ -10510,7 +10510,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30">
+    <row r="3" spans="1:21">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -10674,7 +10674,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1">
-      <c r="A6" s="14"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -10725,7 +10725,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="45">
-      <c r="A7" s="14"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
@@ -10778,7 +10778,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1">
-      <c r="A8" s="14"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -10831,7 +10831,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="45">
-      <c r="A9" s="14"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
@@ -10886,7 +10886,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1">
-      <c r="A10" s="14"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
@@ -10938,8 +10938,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="45">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:21" ht="30">
+      <c r="A11" s="15"/>
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
@@ -10992,7 +10992,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1">
-      <c r="A12" s="14"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -11045,7 +11045,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="75">
-      <c r="A13" s="14"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
@@ -11152,7 +11152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="60">
+    <row r="15" spans="1:21" ht="30">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
         <v>42</v>
@@ -11261,7 +11261,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1">
-      <c r="A17" s="14"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
@@ -11312,7 +11312,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="30">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
@@ -11365,7 +11365,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" customHeight="1">
-      <c r="A19" s="14"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
@@ -11419,8 +11419,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="45">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:21" ht="30">
+      <c r="A20" s="15"/>
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
@@ -11472,7 +11472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="30">
+    <row r="21" spans="1:21">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
         <v>54</v>
@@ -11524,7 +11524,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" customHeight="1">
-      <c r="A22" s="14"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
@@ -11577,7 +11577,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="30">
-      <c r="A23" s="14"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="4" t="s">
         <v>57</v>
       </c>
@@ -11630,7 +11630,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1">
-      <c r="A24" s="14"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="3" t="s">
         <v>59</v>
       </c>
@@ -11683,7 +11683,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="105">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
@@ -11738,7 +11738,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1">
-      <c r="A26" s="14"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
@@ -11791,7 +11791,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="45">
-      <c r="A27" s="14"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
@@ -11846,7 +11846,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1">
-      <c r="A28" s="14"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="3" t="s">
         <v>67</v>
       </c>
@@ -11899,7 +11899,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="60">
-      <c r="A29" s="14"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
@@ -11952,7 +11952,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="30">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
@@ -12058,7 +12058,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
@@ -12113,7 +12113,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="30">
-      <c r="A33" s="14"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="3" t="s">
         <v>77</v>
       </c>
@@ -12221,7 +12221,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="15" customHeight="1">
-      <c r="A35" s="14"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="3" t="s">
         <v>80</v>
       </c>
@@ -12272,7 +12272,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="105">
-      <c r="A36" s="14"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="4" t="s">
         <v>81</v>
       </c>
@@ -12327,7 +12327,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="45">
-      <c r="A37" s="14"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>83</v>
       </c>
@@ -12379,7 +12379,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="60">
+    <row r="38" spans="1:21" ht="45">
       <c r="A38" s="2"/>
       <c r="B38" s="3" t="s">
         <v>84</v>
@@ -12433,7 +12433,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="3" t="s">
         <v>86</v>
       </c>
@@ -12488,7 +12488,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="60">
-      <c r="A40" s="14"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="4" t="s">
         <v>88</v>
       </c>
@@ -12543,7 +12543,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="30">
-      <c r="A41" s="14"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="4" t="s">
         <v>89</v>
       </c>
@@ -12596,7 +12596,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30" customHeight="1">
-      <c r="A42" s="14"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
@@ -12651,7 +12651,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="75">
-      <c r="A43" s="14"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="4" t="s">
         <v>92</v>
       </c>
@@ -12706,7 +12706,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1">
-      <c r="A44" s="14"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
@@ -12761,7 +12761,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="45">
-      <c r="A45" s="14"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="3" t="s">
         <v>96</v>
       </c>
@@ -13140,7 +13140,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" ht="15" customHeight="1">
-      <c r="A52" s="14"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="4" t="s">
         <v>110</v>
       </c>
@@ -13193,7 +13193,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" ht="30">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="3" t="s">
         <v>112</v>
       </c>
@@ -13247,7 +13247,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="30">
+    <row r="54" spans="1:21">
       <c r="A54" s="2"/>
       <c r="B54" s="3" t="s">
         <v>114</v>
@@ -13301,7 +13301,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" ht="60" customHeight="1">
-      <c r="A55" s="14"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="4" t="s">
         <v>116</v>
       </c>
@@ -13356,7 +13356,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" ht="120">
-      <c r="A56" s="14"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="4" t="s">
         <v>119</v>
       </c>
@@ -13411,7 +13411,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" ht="30" customHeight="1">
-      <c r="A57" s="14"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="4" t="s">
         <v>121</v>
       </c>
@@ -13466,7 +13466,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" ht="45">
-      <c r="A58" s="14"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="4" t="s">
         <v>123</v>
       </c>
@@ -13520,7 +13520,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="60">
+    <row r="59" spans="1:21" ht="45">
       <c r="A59" s="2"/>
       <c r="B59" s="3" t="s">
         <v>126</v>
@@ -13573,7 +13573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="60">
+    <row r="60" spans="1:21" ht="45">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
         <v>128</v>
@@ -13629,7 +13629,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="30" customHeight="1">
-      <c r="A61" s="14"/>
+      <c r="A61" s="15"/>
       <c r="B61" s="4" t="s">
         <v>130</v>
       </c>
@@ -13681,8 +13681,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="60">
-      <c r="A62" s="14"/>
+    <row r="62" spans="1:21">
+      <c r="A62" s="15"/>
       <c r="B62" s="4" t="s">
         <v>132</v>
       </c>
@@ -13737,7 +13737,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15" customHeight="1">
-      <c r="A63" s="14"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="3" t="s">
         <v>135</v>
       </c>
@@ -13792,7 +13792,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="75">
-      <c r="A64" s="14"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="4" t="s">
         <v>136</v>
       </c>
@@ -13902,7 +13902,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="45" customHeight="1">
-      <c r="A66" s="14"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="4" t="s">
         <v>139</v>
       </c>
@@ -13957,7 +13957,7 @@
       </c>
     </row>
     <row r="67" spans="1:21" ht="45">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="3" t="s">
         <v>141</v>
       </c>
@@ -14064,7 +14064,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="60">
+    <row r="69" spans="1:21" ht="30">
       <c r="A69" s="2"/>
       <c r="B69" s="4" t="s">
         <v>147</v>
@@ -14118,7 +14118,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" ht="15" customHeight="1">
-      <c r="A70" s="14"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="3" t="s">
         <v>148</v>
       </c>
@@ -14171,7 +14171,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="60">
-      <c r="A71" s="14"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="3" t="s">
         <v>150</v>
       </c>
@@ -14223,8 +14223,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="60">
-      <c r="A72" s="14"/>
+    <row r="72" spans="1:21">
+      <c r="A72" s="15"/>
       <c r="B72" s="3" t="s">
         <v>152</v>
       </c>
@@ -14385,7 +14385,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" ht="15" customHeight="1">
-      <c r="A75" s="14"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="3" t="s">
         <v>157</v>
       </c>
@@ -14438,7 +14438,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" ht="90">
-      <c r="A76" s="14"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="3" t="s">
         <v>158</v>
       </c>
@@ -14493,7 +14493,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" ht="15" customHeight="1">
-      <c r="A77" s="14"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="4" t="s">
         <v>160</v>
       </c>
@@ -14548,7 +14548,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" ht="60">
-      <c r="A78" s="14"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="4" t="s">
         <v>162</v>
       </c>
@@ -14603,7 +14603,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" ht="15" customHeight="1">
-      <c r="A79" s="14"/>
+      <c r="A79" s="15"/>
       <c r="B79" s="4" t="s">
         <v>165</v>
       </c>
@@ -14657,8 +14657,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="45">
-      <c r="A80" s="14"/>
+    <row r="80" spans="1:21" ht="30">
+      <c r="A80" s="15"/>
       <c r="B80" s="4" t="s">
         <v>166</v>
       </c>
@@ -14713,7 +14713,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" ht="45">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="4" t="s">
         <v>168</v>
       </c>
@@ -14764,7 +14764,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" ht="45">
-      <c r="A82" s="14"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="4" t="s">
         <v>170</v>
       </c>
@@ -14817,7 +14817,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" ht="30">
-      <c r="A83" s="14"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="4" t="s">
         <v>171</v>
       </c>
@@ -14980,7 +14980,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="60" customHeight="1">
-      <c r="A86" s="14"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="4" t="s">
         <v>175</v>
       </c>
@@ -15033,7 +15033,7 @@
       </c>
     </row>
     <row r="87" spans="1:21">
-      <c r="A87" s="14"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="4" t="s">
         <v>176</v>
       </c>
@@ -15086,7 +15086,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="75" customHeight="1">
-      <c r="A88" s="14"/>
+      <c r="A88" s="15"/>
       <c r="B88" s="3" t="s">
         <v>177</v>
       </c>
@@ -15141,7 +15141,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" ht="45">
-      <c r="A89" s="14"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="4" t="s">
         <v>178</v>
       </c>
@@ -15194,7 +15194,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" ht="30" customHeight="1">
-      <c r="A90" s="14"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="4" t="s">
         <v>180</v>
       </c>
@@ -15247,7 +15247,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" ht="30">
-      <c r="A91" s="14"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="4" t="s">
         <v>182</v>
       </c>
@@ -15298,7 +15298,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" ht="15" customHeight="1">
-      <c r="A92" s="14"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="4" t="s">
         <v>184</v>
       </c>
@@ -15352,8 +15352,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="30">
-      <c r="A93" s="14"/>
+    <row r="93" spans="1:21">
+      <c r="A93" s="15"/>
       <c r="B93" s="3" t="s">
         <v>185</v>
       </c>
@@ -15458,7 +15458,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="60">
+    <row r="95" spans="1:21" ht="45">
       <c r="A95" s="2"/>
       <c r="B95" s="3" t="s">
         <v>189</v>
@@ -15510,7 +15510,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" ht="15" customHeight="1">
-      <c r="A96" s="14"/>
+      <c r="A96" s="15"/>
       <c r="B96" s="3" t="s">
         <v>191</v>
       </c>
@@ -15563,7 +15563,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" ht="30">
-      <c r="A97" s="14"/>
+      <c r="A97" s="15"/>
       <c r="B97" s="3" t="s">
         <v>192</v>
       </c>
@@ -15618,7 +15618,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" ht="15" customHeight="1">
-      <c r="A98" s="14"/>
+      <c r="A98" s="15"/>
       <c r="B98" s="4" t="s">
         <v>193</v>
       </c>
@@ -15673,7 +15673,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" ht="45">
-      <c r="A99" s="14"/>
+      <c r="A99" s="15"/>
       <c r="B99" s="4" t="s">
         <v>194</v>
       </c>
@@ -15725,7 +15725,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:21" ht="45">
+    <row r="100" spans="1:21" ht="30">
       <c r="A100" s="2"/>
       <c r="B100" s="3" t="s">
         <v>195</v>
@@ -15779,7 +15779,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" ht="15" customHeight="1">
-      <c r="A101" s="14"/>
+      <c r="A101" s="15"/>
       <c r="B101" s="3" t="s">
         <v>196</v>
       </c>
@@ -15834,7 +15834,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="60">
-      <c r="A102" s="14"/>
+      <c r="A102" s="15"/>
       <c r="B102" s="3" t="s">
         <v>197</v>
       </c>
@@ -15889,7 +15889,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" ht="15" customHeight="1">
-      <c r="A103" s="14"/>
+      <c r="A103" s="15"/>
       <c r="B103" s="4" t="s">
         <v>198</v>
       </c>
@@ -15943,8 +15943,8 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:21" ht="45">
-      <c r="A104" s="14"/>
+    <row r="104" spans="1:21" ht="30">
+      <c r="A104" s="15"/>
       <c r="B104" s="4" t="s">
         <v>199</v>
       </c>
@@ -15997,7 +15997,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="15" customHeight="1">
-      <c r="A105" s="14"/>
+      <c r="A105" s="15"/>
       <c r="B105" s="3" t="s">
         <v>200</v>
       </c>
@@ -16050,7 +16050,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="45">
-      <c r="A106" s="14"/>
+      <c r="A106" s="15"/>
       <c r="B106" s="4" t="s">
         <v>202</v>
       </c>
@@ -16154,7 +16154,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" ht="15" customHeight="1">
-      <c r="A108" s="14"/>
+      <c r="A108" s="15"/>
       <c r="B108" s="3" t="s">
         <v>204</v>
       </c>
@@ -16204,8 +16204,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="75">
-      <c r="A109" s="14"/>
+    <row r="109" spans="1:21" ht="60">
+      <c r="A109" s="15"/>
       <c r="B109" s="3" t="s">
         <v>206</v>
       </c>
@@ -16258,7 +16258,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="30">
-      <c r="A110" s="14"/>
+      <c r="A110" s="15"/>
       <c r="B110" s="4" t="s">
         <v>208</v>
       </c>
@@ -16311,7 +16311,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="15" customHeight="1">
-      <c r="A111" s="14"/>
+      <c r="A111" s="15"/>
       <c r="B111" s="4" t="s">
         <v>209</v>
       </c>
@@ -16361,8 +16361,8 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:21" ht="45">
-      <c r="A112" s="14"/>
+    <row r="112" spans="1:21" ht="30">
+      <c r="A112" s="15"/>
       <c r="B112" s="4" t="s">
         <v>211</v>
       </c>
@@ -16467,7 +16467,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:21" ht="45">
+    <row r="114" spans="1:21" ht="30">
       <c r="A114" s="2"/>
       <c r="B114" s="4" t="s">
         <v>214</v>
@@ -16627,7 +16627,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" ht="15" customHeight="1">
-      <c r="A117" s="14"/>
+      <c r="A117" s="15"/>
       <c r="B117" s="4" t="s">
         <v>220</v>
       </c>
@@ -16682,7 +16682,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" ht="105">
-      <c r="A118" s="14"/>
+      <c r="A118" s="15"/>
       <c r="B118" s="4" t="s">
         <v>221</v>
       </c>
@@ -16841,7 +16841,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" ht="15" customHeight="1">
-      <c r="A121" s="14"/>
+      <c r="A121" s="15"/>
       <c r="B121" s="4"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -16853,72 +16853,72 @@
       <c r="M121" s="4"/>
     </row>
     <row r="122" spans="1:21">
-      <c r="A122" s="14"/>
+      <c r="A122" s="15"/>
       <c r="I122" s="4"/>
       <c r="M122" s="4"/>
     </row>
     <row r="123" spans="1:21" ht="15" customHeight="1">
-      <c r="A123" s="14"/>
+      <c r="A123" s="15"/>
       <c r="I123" s="4"/>
       <c r="M123" s="4"/>
     </row>
     <row r="124" spans="1:21">
-      <c r="A124" s="14"/>
+      <c r="A124" s="15"/>
       <c r="I124" s="4"/>
       <c r="M124" s="4"/>
     </row>
     <row r="125" spans="1:21" ht="15" customHeight="1">
-      <c r="A125" s="14"/>
+      <c r="A125" s="15"/>
       <c r="I125" s="4"/>
       <c r="M125" s="4"/>
     </row>
     <row r="126" spans="1:21">
-      <c r="A126" s="14"/>
+      <c r="A126" s="15"/>
       <c r="I126" s="4"/>
       <c r="M126" s="4"/>
     </row>
     <row r="127" spans="1:21">
-      <c r="A127" s="14"/>
+      <c r="A127" s="15"/>
       <c r="I127" s="4"/>
       <c r="M127" s="4"/>
     </row>
     <row r="128" spans="1:21" ht="15" customHeight="1">
-      <c r="A128" s="14"/>
+      <c r="A128" s="15"/>
       <c r="I128" s="4"/>
       <c r="M128" s="4"/>
     </row>
     <row r="129" spans="1:13">
-      <c r="A129" s="14"/>
+      <c r="A129" s="15"/>
       <c r="I129" s="4"/>
       <c r="M129" s="4"/>
     </row>
     <row r="130" spans="1:13" ht="15" customHeight="1">
-      <c r="A130" s="14"/>
+      <c r="A130" s="15"/>
       <c r="I130" s="4"/>
       <c r="M130" s="4"/>
     </row>
     <row r="131" spans="1:13">
-      <c r="A131" s="14"/>
+      <c r="A131" s="15"/>
       <c r="I131" s="4"/>
       <c r="M131" s="4"/>
     </row>
     <row r="132" spans="1:13" ht="15" customHeight="1">
-      <c r="A132" s="14"/>
+      <c r="A132" s="15"/>
       <c r="I132" s="4"/>
       <c r="M132" s="4"/>
     </row>
     <row r="133" spans="1:13">
-      <c r="A133" s="14"/>
+      <c r="A133" s="15"/>
       <c r="I133" s="4"/>
       <c r="M133" s="4"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
-      <c r="A134" s="14"/>
+      <c r="A134" s="15"/>
       <c r="I134" s="4"/>
       <c r="M134" s="4"/>
     </row>
     <row r="135" spans="1:13">
-      <c r="A135" s="14"/>
+      <c r="A135" s="15"/>
       <c r="I135" s="4"/>
       <c r="M135" s="4"/>
     </row>
@@ -16933,22 +16933,22 @@
       <c r="M137" s="4"/>
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1">
-      <c r="A138" s="14"/>
+      <c r="A138" s="15"/>
       <c r="I138" s="4"/>
       <c r="M138" s="4"/>
     </row>
     <row r="139" spans="1:13">
-      <c r="A139" s="14"/>
+      <c r="A139" s="15"/>
       <c r="I139" s="4"/>
       <c r="M139" s="4"/>
     </row>
     <row r="140" spans="1:13">
-      <c r="A140" s="14"/>
+      <c r="A140" s="15"/>
       <c r="I140" s="4"/>
       <c r="M140" s="4"/>
     </row>
     <row r="141" spans="1:13">
-      <c r="A141" s="14"/>
+      <c r="A141" s="15"/>
       <c r="I141" s="4"/>
       <c r="M141" s="4"/>
     </row>
@@ -16958,47 +16958,47 @@
       <c r="M142" s="4"/>
     </row>
     <row r="143" spans="1:13" ht="15" customHeight="1">
-      <c r="A143" s="14"/>
+      <c r="A143" s="15"/>
       <c r="I143" s="4"/>
       <c r="M143" s="4"/>
     </row>
     <row r="144" spans="1:13">
-      <c r="A144" s="14"/>
+      <c r="A144" s="15"/>
       <c r="I144" s="4"/>
       <c r="M144" s="4"/>
     </row>
     <row r="145" spans="1:13" ht="15" customHeight="1">
-      <c r="A145" s="14"/>
+      <c r="A145" s="15"/>
       <c r="I145" s="4"/>
       <c r="M145" s="4"/>
     </row>
     <row r="146" spans="1:13">
-      <c r="A146" s="14"/>
+      <c r="A146" s="15"/>
       <c r="I146" s="4"/>
       <c r="M146" s="4"/>
     </row>
     <row r="147" spans="1:13">
-      <c r="A147" s="14"/>
+      <c r="A147" s="15"/>
       <c r="I147" s="4"/>
       <c r="M147" s="4"/>
     </row>
     <row r="148" spans="1:13" ht="15" customHeight="1">
-      <c r="A148" s="14"/>
+      <c r="A148" s="15"/>
       <c r="I148" s="4"/>
       <c r="M148" s="4"/>
     </row>
     <row r="149" spans="1:13">
-      <c r="A149" s="14"/>
+      <c r="A149" s="15"/>
       <c r="I149" s="4"/>
       <c r="M149" s="4"/>
     </row>
     <row r="150" spans="1:13" ht="45" customHeight="1">
-      <c r="A150" s="14"/>
+      <c r="A150" s="15"/>
       <c r="I150" s="4"/>
       <c r="M150" s="4"/>
     </row>
     <row r="151" spans="1:13">
-      <c r="A151" s="14"/>
+      <c r="A151" s="15"/>
       <c r="I151" s="4"/>
       <c r="M151" s="4"/>
     </row>
@@ -17028,22 +17028,22 @@
       <c r="M156" s="4"/>
     </row>
     <row r="157" spans="1:13" ht="15" customHeight="1">
-      <c r="A157" s="14"/>
+      <c r="A157" s="15"/>
       <c r="I157" s="4"/>
       <c r="M157" s="4"/>
     </row>
     <row r="158" spans="1:13">
-      <c r="A158" s="14"/>
+      <c r="A158" s="15"/>
       <c r="I158" s="4"/>
       <c r="M158" s="4"/>
     </row>
     <row r="159" spans="1:13" ht="15" customHeight="1">
-      <c r="A159" s="14"/>
+      <c r="A159" s="15"/>
       <c r="I159" s="4"/>
       <c r="M159" s="4"/>
     </row>
     <row r="160" spans="1:13">
-      <c r="A160" s="14"/>
+      <c r="A160" s="15"/>
       <c r="I160" s="4"/>
       <c r="M160" s="4"/>
     </row>
@@ -17063,22 +17063,22 @@
       <c r="M163" s="4"/>
     </row>
     <row r="164" spans="1:13" ht="15" customHeight="1">
-      <c r="A164" s="14"/>
+      <c r="A164" s="15"/>
       <c r="I164" s="4"/>
       <c r="M164" s="4"/>
     </row>
     <row r="165" spans="1:13">
-      <c r="A165" s="14"/>
+      <c r="A165" s="15"/>
       <c r="I165" s="4"/>
       <c r="M165" s="4"/>
     </row>
     <row r="166" spans="1:13" ht="15" customHeight="1">
-      <c r="A166" s="14"/>
+      <c r="A166" s="15"/>
       <c r="I166" s="4"/>
       <c r="M166" s="4"/>
     </row>
     <row r="167" spans="1:13">
-      <c r="A167" s="14"/>
+      <c r="A167" s="15"/>
       <c r="I167" s="4"/>
       <c r="M167" s="4"/>
     </row>
@@ -17088,12 +17088,12 @@
       <c r="M168" s="4"/>
     </row>
     <row r="169" spans="1:13" ht="15" customHeight="1">
-      <c r="A169" s="14"/>
+      <c r="A169" s="15"/>
       <c r="I169" s="4"/>
       <c r="M169" s="4"/>
     </row>
     <row r="170" spans="1:13">
-      <c r="A170" s="14"/>
+      <c r="A170" s="15"/>
       <c r="I170" s="4"/>
       <c r="M170" s="4"/>
     </row>
@@ -17113,67 +17113,67 @@
       <c r="M173" s="4"/>
     </row>
     <row r="174" spans="1:13" ht="15" customHeight="1">
-      <c r="A174" s="14"/>
+      <c r="A174" s="15"/>
       <c r="I174" s="4"/>
       <c r="M174" s="4"/>
     </row>
     <row r="175" spans="1:13">
-      <c r="A175" s="14"/>
+      <c r="A175" s="15"/>
       <c r="I175" s="4"/>
       <c r="M175" s="4"/>
     </row>
     <row r="176" spans="1:13" ht="15" customHeight="1">
-      <c r="A176" s="14"/>
+      <c r="A176" s="15"/>
       <c r="I176" s="4"/>
       <c r="M176" s="4"/>
     </row>
     <row r="177" spans="1:13">
-      <c r="A177" s="14"/>
+      <c r="A177" s="15"/>
       <c r="I177" s="4"/>
       <c r="M177" s="4"/>
     </row>
     <row r="178" spans="1:13">
-      <c r="A178" s="14"/>
+      <c r="A178" s="15"/>
       <c r="I178" s="4"/>
       <c r="M178" s="4"/>
     </row>
     <row r="179" spans="1:13" ht="15" customHeight="1">
-      <c r="A179" s="14"/>
+      <c r="A179" s="15"/>
       <c r="I179" s="4"/>
       <c r="M179" s="4"/>
     </row>
     <row r="180" spans="1:13">
-      <c r="A180" s="14"/>
+      <c r="A180" s="15"/>
       <c r="I180" s="4"/>
       <c r="M180" s="4"/>
     </row>
     <row r="181" spans="1:13" ht="15" customHeight="1">
-      <c r="A181" s="14"/>
+      <c r="A181" s="15"/>
       <c r="I181" s="4"/>
       <c r="M181" s="4"/>
     </row>
     <row r="182" spans="1:13">
-      <c r="A182" s="14"/>
+      <c r="A182" s="15"/>
       <c r="I182" s="4"/>
       <c r="M182" s="4"/>
     </row>
     <row r="183" spans="1:13" ht="15" customHeight="1">
-      <c r="A183" s="14"/>
+      <c r="A183" s="15"/>
       <c r="I183" s="4"/>
       <c r="M183" s="4"/>
     </row>
     <row r="184" spans="1:13">
-      <c r="A184" s="14"/>
+      <c r="A184" s="15"/>
       <c r="I184" s="4"/>
       <c r="M184" s="4"/>
     </row>
     <row r="185" spans="1:13" ht="15" customHeight="1">
-      <c r="A185" s="14"/>
+      <c r="A185" s="15"/>
       <c r="I185" s="4"/>
       <c r="M185" s="4"/>
     </row>
     <row r="186" spans="1:13">
-      <c r="A186" s="14"/>
+      <c r="A186" s="15"/>
       <c r="I186" s="4"/>
       <c r="M186" s="4"/>
     </row>
@@ -17183,22 +17183,22 @@
       <c r="M187" s="4"/>
     </row>
     <row r="188" spans="1:13" ht="15" customHeight="1">
-      <c r="A188" s="14"/>
+      <c r="A188" s="15"/>
       <c r="I188" s="4"/>
       <c r="M188" s="4"/>
     </row>
     <row r="189" spans="1:13">
-      <c r="A189" s="14"/>
+      <c r="A189" s="15"/>
       <c r="I189" s="4"/>
       <c r="M189" s="4"/>
     </row>
     <row r="190" spans="1:13" ht="60" customHeight="1">
-      <c r="A190" s="14"/>
+      <c r="A190" s="15"/>
       <c r="I190" s="4"/>
       <c r="M190" s="4"/>
     </row>
     <row r="191" spans="1:13">
-      <c r="A191" s="14"/>
+      <c r="A191" s="15"/>
       <c r="I191" s="4"/>
       <c r="M191" s="4"/>
     </row>
@@ -17208,12 +17208,12 @@
       <c r="M192" s="4"/>
     </row>
     <row r="193" spans="1:13" ht="45" customHeight="1">
-      <c r="A193" s="14"/>
+      <c r="A193" s="15"/>
       <c r="I193" s="4"/>
       <c r="M193" s="4"/>
     </row>
     <row r="194" spans="1:13">
-      <c r="A194" s="14"/>
+      <c r="A194" s="15"/>
       <c r="I194" s="4"/>
       <c r="M194" s="4"/>
     </row>
@@ -17222,6 +17222,58 @@
     <sortCondition ref="T1:T232"/>
   </sortState>
   <mergeCells count="68">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="A138:A139"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="A193:A194"/>
     <mergeCell ref="A190:A191"/>
@@ -17238,58 +17290,6 @@
     <mergeCell ref="A159:A160"/>
     <mergeCell ref="A157:A158"/>
     <mergeCell ref="A150:A151"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" tooltip="Absolute Zero" display="http://crawl.chaosforge.org/Absolute_Zero" xr:uid="{0B7D80AD-41C3-4378-86E9-351B477A2B9F}"/>
@@ -17480,7 +17480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E8B271-C60B-40E0-8071-44B09290B0A0}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -18668,13 +18668,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E9C651-19A5-494D-8095-C1365B59BB3C}">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="55.28515625" customWidth="1"/>

</xml_diff>

<commit_message>
added code to parse player abilities from menu text
</commit_message>
<xml_diff>
--- a/models/wiki_data_manually_entered.xlsx
+++ b/models/wiki_data_manually_entered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bbe28fe5e73b7d58/Code Projects/dcss-ai-wrapper/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E74E18A-B48C-4FE2-BBB2-AFB0697115CB}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{4B1E9A8A-F23B-4E52-8155-A40DE090198E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2C4FDB4-B06E-4854-A1A6-4FCE26BBA9EB}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="3390" windowWidth="28170" windowHeight="15435" activeTab="3" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
+    <workbookView xWindow="18360" yWindow="3390" windowWidth="31110" windowHeight="15405" activeTab="3" xr2:uid="{5C052992-BA14-4E63-B755-78C10F0D6DBE}"/>
   </bookViews>
   <sheets>
     <sheet name="spells" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="898">
   <si>
     <t>Icon</t>
   </si>
@@ -2673,6 +2673,210 @@
   </si>
   <si>
     <t>r*2</t>
+  </si>
+  <si>
+    <t>spit poison</t>
+  </si>
+  <si>
+    <t>heal wounds</t>
+  </si>
+  <si>
+    <t>rolling charge</t>
+  </si>
+  <si>
+    <t>bat form</t>
+  </si>
+  <si>
+    <t>curse item</t>
+  </si>
+  <si>
+    <t>transfer knowledge</t>
+  </si>
+  <si>
+    <t>give item to follower</t>
+  </si>
+  <si>
+    <t>bend time</t>
+  </si>
+  <si>
+    <t>temporal distortion</t>
+  </si>
+  <si>
+    <t>step from time</t>
+  </si>
+  <si>
+    <t>shadow step</t>
+  </si>
+  <si>
+    <t>shadow form</t>
+  </si>
+  <si>
+    <t>lesser healing</t>
+  </si>
+  <si>
+    <t>divine protection</t>
+  </si>
+  <si>
+    <t>heal other</t>
+  </si>
+  <si>
+    <t>controlled blink</t>
+  </si>
+  <si>
+    <t>greater healing</t>
+  </si>
+  <si>
+    <t>divine vigour</t>
+  </si>
+  <si>
+    <t>briar patch</t>
+  </si>
+  <si>
+    <t>grow ballistomycete</t>
+  </si>
+  <si>
+    <t>grow oklob plant</t>
+  </si>
+  <si>
+    <t>potion petition</t>
+  </si>
+  <si>
+    <t>call merchant</t>
+  </si>
+  <si>
+    <t>bribe branch</t>
+  </si>
+  <si>
+    <t>ancestor identity</t>
+  </si>
+  <si>
+    <t>ancestor life</t>
+  </si>
+  <si>
+    <t>request jelly</t>
+  </si>
+  <si>
+    <t>gain random mutations</t>
+  </si>
+  <si>
+    <t>cure bad mutations</t>
+  </si>
+  <si>
+    <t>receive corpses</t>
+  </si>
+  <si>
+    <t>receive necronomicon</t>
+  </si>
+  <si>
+    <t>brand weapon with pain</t>
+  </si>
+  <si>
+    <t>depart abyss</t>
+  </si>
+  <si>
+    <t>bend space</t>
+  </si>
+  <si>
+    <t>banish self</t>
+  </si>
+  <si>
+    <t>corrupt weapon</t>
+  </si>
+  <si>
+    <t>minor destruction</t>
+  </si>
+  <si>
+    <t>summon lesser servant</t>
+  </si>
+  <si>
+    <t>major destruction</t>
+  </si>
+  <si>
+    <t>summon greater servant</t>
+  </si>
+  <si>
+    <t>pick a card any card</t>
+  </si>
+  <si>
+    <t>triple draw</t>
+  </si>
+  <si>
+    <t>deal four</t>
+  </si>
+  <si>
+    <t>stack five</t>
+  </si>
+  <si>
+    <t>elemental force</t>
+  </si>
+  <si>
+    <t>disaster area</t>
+  </si>
+  <si>
+    <t>draw out power</t>
+  </si>
+  <si>
+    <t>power leap</t>
+  </si>
+  <si>
+    <t>toggle divine energy</t>
+  </si>
+  <si>
+    <t>channel magic</t>
+  </si>
+  <si>
+    <t>forget spell</t>
+  </si>
+  <si>
+    <t>trogs hand</t>
+  </si>
+  <si>
+    <t>brothers in arms</t>
+  </si>
+  <si>
+    <t>line pass</t>
+  </si>
+  <si>
+    <t>grand finale</t>
+  </si>
+  <si>
+    <t>wall jump</t>
+  </si>
+  <si>
+    <t>serpents lash</t>
+  </si>
+  <si>
+    <t>heavenly storm</t>
+  </si>
+  <si>
+    <t>animate remains</t>
+  </si>
+  <si>
+    <t>toggle injury mirror</t>
+  </si>
+  <si>
+    <t>recall undead slaves</t>
+  </si>
+  <si>
+    <t>animate dead</t>
+  </si>
+  <si>
+    <t>drain life</t>
+  </si>
+  <si>
+    <t>enslave soul</t>
+  </si>
+  <si>
+    <t>divine shield</t>
+  </si>
+  <si>
+    <t>cleansing flame</t>
+  </si>
+  <si>
+    <t>summon divine warrior</t>
+  </si>
+  <si>
+    <t>brand weapon with holy</t>
   </si>
 </sst>
 </file>
@@ -2791,11 +2995,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10452,7 +10656,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -10476,8 +10680,8 @@
       <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="I1" s="15"/>
+      <c r="M1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="T1" t="s">
@@ -10485,7 +10689,7 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="14"/>
+      <c r="A2" s="15"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -10495,8 +10699,8 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="M2" s="15"/>
       <c r="P2" s="8" t="s">
         <v>227</v>
       </c>
@@ -10674,7 +10878,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
@@ -10725,7 +10929,7 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="45">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
@@ -10778,7 +10982,7 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" customHeight="1">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
@@ -10831,7 +11035,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="45">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
@@ -10886,7 +11090,7 @@
       </c>
     </row>
     <row r="10" spans="1:21" ht="15" customHeight="1">
-      <c r="A10" s="15"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
@@ -10939,7 +11143,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="30">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
@@ -10992,7 +11196,7 @@
       </c>
     </row>
     <row r="12" spans="1:21" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
@@ -11045,7 +11249,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" ht="75">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="4" t="s">
         <v>37</v>
       </c>
@@ -11261,7 +11465,7 @@
       </c>
     </row>
     <row r="17" spans="1:21" ht="15" customHeight="1">
-      <c r="A17" s="15"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
@@ -11312,7 +11516,7 @@
       </c>
     </row>
     <row r="18" spans="1:21" ht="30">
-      <c r="A18" s="15"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="4" t="s">
         <v>46</v>
       </c>
@@ -11365,7 +11569,7 @@
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" customHeight="1">
-      <c r="A19" s="15"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
@@ -11420,7 +11624,7 @@
       </c>
     </row>
     <row r="20" spans="1:21" ht="30">
-      <c r="A20" s="15"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="3" t="s">
         <v>51</v>
       </c>
@@ -11524,7 +11728,7 @@
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" customHeight="1">
-      <c r="A22" s="15"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="3" t="s">
         <v>55</v>
       </c>
@@ -11577,7 +11781,7 @@
       </c>
     </row>
     <row r="23" spans="1:21" ht="30">
-      <c r="A23" s="15"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="4" t="s">
         <v>57</v>
       </c>
@@ -11630,7 +11834,7 @@
       </c>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1">
-      <c r="A24" s="15"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="3" t="s">
         <v>59</v>
       </c>
@@ -11683,7 +11887,7 @@
       </c>
     </row>
     <row r="25" spans="1:21" ht="105">
-      <c r="A25" s="15"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="4" t="s">
         <v>61</v>
       </c>
@@ -11738,7 +11942,7 @@
       </c>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1">
-      <c r="A26" s="15"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="4" t="s">
         <v>62</v>
       </c>
@@ -11791,7 +11995,7 @@
       </c>
     </row>
     <row r="27" spans="1:21" ht="45">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="4" t="s">
         <v>64</v>
       </c>
@@ -11846,7 +12050,7 @@
       </c>
     </row>
     <row r="28" spans="1:21" ht="15" customHeight="1">
-      <c r="A28" s="15"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3" t="s">
         <v>67</v>
       </c>
@@ -11899,7 +12103,7 @@
       </c>
     </row>
     <row r="29" spans="1:21" ht="60">
-      <c r="A29" s="15"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="3" t="s">
         <v>69</v>
       </c>
@@ -11952,7 +12156,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" ht="30">
-      <c r="A30" s="15"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
@@ -12058,7 +12262,7 @@
       </c>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1">
-      <c r="A32" s="15"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="3" t="s">
         <v>76</v>
       </c>
@@ -12113,7 +12317,7 @@
       </c>
     </row>
     <row r="33" spans="1:21" ht="30">
-      <c r="A33" s="15"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="3" t="s">
         <v>77</v>
       </c>
@@ -12221,7 +12425,7 @@
       </c>
     </row>
     <row r="35" spans="1:21" ht="15" customHeight="1">
-      <c r="A35" s="15"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="3" t="s">
         <v>80</v>
       </c>
@@ -12272,7 +12476,7 @@
       </c>
     </row>
     <row r="36" spans="1:21" ht="105">
-      <c r="A36" s="15"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="4" t="s">
         <v>81</v>
       </c>
@@ -12327,7 +12531,7 @@
       </c>
     </row>
     <row r="37" spans="1:21" ht="45">
-      <c r="A37" s="15"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="4" t="s">
         <v>83</v>
       </c>
@@ -12433,7 +12637,7 @@
       </c>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1">
-      <c r="A39" s="15"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="3" t="s">
         <v>86</v>
       </c>
@@ -12488,7 +12692,7 @@
       </c>
     </row>
     <row r="40" spans="1:21" ht="60">
-      <c r="A40" s="15"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="4" t="s">
         <v>88</v>
       </c>
@@ -12543,7 +12747,7 @@
       </c>
     </row>
     <row r="41" spans="1:21" ht="30">
-      <c r="A41" s="15"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="4" t="s">
         <v>89</v>
       </c>
@@ -12596,7 +12800,7 @@
       </c>
     </row>
     <row r="42" spans="1:21" ht="30" customHeight="1">
-      <c r="A42" s="15"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="3" t="s">
         <v>90</v>
       </c>
@@ -12651,7 +12855,7 @@
       </c>
     </row>
     <row r="43" spans="1:21" ht="75">
-      <c r="A43" s="15"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="4" t="s">
         <v>92</v>
       </c>
@@ -12706,7 +12910,7 @@
       </c>
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1">
-      <c r="A44" s="15"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
@@ -12761,7 +12965,7 @@
       </c>
     </row>
     <row r="45" spans="1:21" ht="45">
-      <c r="A45" s="15"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="3" t="s">
         <v>96</v>
       </c>
@@ -13140,7 +13344,7 @@
       </c>
     </row>
     <row r="52" spans="1:21" ht="15" customHeight="1">
-      <c r="A52" s="15"/>
+      <c r="A52" s="14"/>
       <c r="B52" s="4" t="s">
         <v>110</v>
       </c>
@@ -13193,7 +13397,7 @@
       </c>
     </row>
     <row r="53" spans="1:21" ht="30">
-      <c r="A53" s="15"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="3" t="s">
         <v>112</v>
       </c>
@@ -13301,7 +13505,7 @@
       </c>
     </row>
     <row r="55" spans="1:21" ht="60" customHeight="1">
-      <c r="A55" s="15"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="4" t="s">
         <v>116</v>
       </c>
@@ -13356,7 +13560,7 @@
       </c>
     </row>
     <row r="56" spans="1:21" ht="120">
-      <c r="A56" s="15"/>
+      <c r="A56" s="14"/>
       <c r="B56" s="4" t="s">
         <v>119</v>
       </c>
@@ -13411,7 +13615,7 @@
       </c>
     </row>
     <row r="57" spans="1:21" ht="30" customHeight="1">
-      <c r="A57" s="15"/>
+      <c r="A57" s="14"/>
       <c r="B57" s="4" t="s">
         <v>121</v>
       </c>
@@ -13466,7 +13670,7 @@
       </c>
     </row>
     <row r="58" spans="1:21" ht="45">
-      <c r="A58" s="15"/>
+      <c r="A58" s="14"/>
       <c r="B58" s="4" t="s">
         <v>123</v>
       </c>
@@ -13629,7 +13833,7 @@
       </c>
     </row>
     <row r="61" spans="1:21" ht="30" customHeight="1">
-      <c r="A61" s="15"/>
+      <c r="A61" s="14"/>
       <c r="B61" s="4" t="s">
         <v>130</v>
       </c>
@@ -13682,7 +13886,7 @@
       </c>
     </row>
     <row r="62" spans="1:21">
-      <c r="A62" s="15"/>
+      <c r="A62" s="14"/>
       <c r="B62" s="4" t="s">
         <v>132</v>
       </c>
@@ -13737,7 +13941,7 @@
       </c>
     </row>
     <row r="63" spans="1:21" ht="15" customHeight="1">
-      <c r="A63" s="15"/>
+      <c r="A63" s="14"/>
       <c r="B63" s="3" t="s">
         <v>135</v>
       </c>
@@ -13792,7 +13996,7 @@
       </c>
     </row>
     <row r="64" spans="1:21" ht="75">
-      <c r="A64" s="15"/>
+      <c r="A64" s="14"/>
       <c r="B64" s="4" t="s">
         <v>136</v>
       </c>
@@ -13902,7 +14106,7 @@
       </c>
     </row>
     <row r="66" spans="1:21" ht="45" customHeight="1">
-      <c r="A66" s="15"/>
+      <c r="A66" s="14"/>
       <c r="B66" s="4" t="s">
         <v>139</v>
       </c>
@@ -13957,7 +14161,7 @@
       </c>
     </row>
     <row r="67" spans="1:21" ht="45">
-      <c r="A67" s="15"/>
+      <c r="A67" s="14"/>
       <c r="B67" s="3" t="s">
         <v>141</v>
       </c>
@@ -14118,7 +14322,7 @@
       </c>
     </row>
     <row r="70" spans="1:21" ht="15" customHeight="1">
-      <c r="A70" s="15"/>
+      <c r="A70" s="14"/>
       <c r="B70" s="3" t="s">
         <v>148</v>
       </c>
@@ -14171,7 +14375,7 @@
       </c>
     </row>
     <row r="71" spans="1:21" ht="60">
-      <c r="A71" s="15"/>
+      <c r="A71" s="14"/>
       <c r="B71" s="3" t="s">
         <v>150</v>
       </c>
@@ -14224,7 +14428,7 @@
       </c>
     </row>
     <row r="72" spans="1:21">
-      <c r="A72" s="15"/>
+      <c r="A72" s="14"/>
       <c r="B72" s="3" t="s">
         <v>152</v>
       </c>
@@ -14385,7 +14589,7 @@
       </c>
     </row>
     <row r="75" spans="1:21" ht="15" customHeight="1">
-      <c r="A75" s="15"/>
+      <c r="A75" s="14"/>
       <c r="B75" s="3" t="s">
         <v>157</v>
       </c>
@@ -14438,7 +14642,7 @@
       </c>
     </row>
     <row r="76" spans="1:21" ht="90">
-      <c r="A76" s="15"/>
+      <c r="A76" s="14"/>
       <c r="B76" s="3" t="s">
         <v>158</v>
       </c>
@@ -14493,7 +14697,7 @@
       </c>
     </row>
     <row r="77" spans="1:21" ht="15" customHeight="1">
-      <c r="A77" s="15"/>
+      <c r="A77" s="14"/>
       <c r="B77" s="4" t="s">
         <v>160</v>
       </c>
@@ -14548,7 +14752,7 @@
       </c>
     </row>
     <row r="78" spans="1:21" ht="60">
-      <c r="A78" s="15"/>
+      <c r="A78" s="14"/>
       <c r="B78" s="4" t="s">
         <v>162</v>
       </c>
@@ -14603,7 +14807,7 @@
       </c>
     </row>
     <row r="79" spans="1:21" ht="15" customHeight="1">
-      <c r="A79" s="15"/>
+      <c r="A79" s="14"/>
       <c r="B79" s="4" t="s">
         <v>165</v>
       </c>
@@ -14658,7 +14862,7 @@
       </c>
     </row>
     <row r="80" spans="1:21" ht="30">
-      <c r="A80" s="15"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="4" t="s">
         <v>166</v>
       </c>
@@ -14713,7 +14917,7 @@
       </c>
     </row>
     <row r="81" spans="1:21" ht="45">
-      <c r="A81" s="15"/>
+      <c r="A81" s="14"/>
       <c r="B81" s="4" t="s">
         <v>168</v>
       </c>
@@ -14764,7 +14968,7 @@
       </c>
     </row>
     <row r="82" spans="1:21" ht="45">
-      <c r="A82" s="15"/>
+      <c r="A82" s="14"/>
       <c r="B82" s="4" t="s">
         <v>170</v>
       </c>
@@ -14817,7 +15021,7 @@
       </c>
     </row>
     <row r="83" spans="1:21" ht="30">
-      <c r="A83" s="15"/>
+      <c r="A83" s="14"/>
       <c r="B83" s="4" t="s">
         <v>171</v>
       </c>
@@ -14980,7 +15184,7 @@
       </c>
     </row>
     <row r="86" spans="1:21" ht="60" customHeight="1">
-      <c r="A86" s="15"/>
+      <c r="A86" s="14"/>
       <c r="B86" s="4" t="s">
         <v>175</v>
       </c>
@@ -15033,7 +15237,7 @@
       </c>
     </row>
     <row r="87" spans="1:21">
-      <c r="A87" s="15"/>
+      <c r="A87" s="14"/>
       <c r="B87" s="4" t="s">
         <v>176</v>
       </c>
@@ -15086,7 +15290,7 @@
       </c>
     </row>
     <row r="88" spans="1:21" ht="75" customHeight="1">
-      <c r="A88" s="15"/>
+      <c r="A88" s="14"/>
       <c r="B88" s="3" t="s">
         <v>177</v>
       </c>
@@ -15141,7 +15345,7 @@
       </c>
     </row>
     <row r="89" spans="1:21" ht="45">
-      <c r="A89" s="15"/>
+      <c r="A89" s="14"/>
       <c r="B89" s="4" t="s">
         <v>178</v>
       </c>
@@ -15194,7 +15398,7 @@
       </c>
     </row>
     <row r="90" spans="1:21" ht="30" customHeight="1">
-      <c r="A90" s="15"/>
+      <c r="A90" s="14"/>
       <c r="B90" s="4" t="s">
         <v>180</v>
       </c>
@@ -15247,7 +15451,7 @@
       </c>
     </row>
     <row r="91" spans="1:21" ht="30">
-      <c r="A91" s="15"/>
+      <c r="A91" s="14"/>
       <c r="B91" s="4" t="s">
         <v>182</v>
       </c>
@@ -15298,7 +15502,7 @@
       </c>
     </row>
     <row r="92" spans="1:21" ht="15" customHeight="1">
-      <c r="A92" s="15"/>
+      <c r="A92" s="14"/>
       <c r="B92" s="4" t="s">
         <v>184</v>
       </c>
@@ -15353,7 +15557,7 @@
       </c>
     </row>
     <row r="93" spans="1:21">
-      <c r="A93" s="15"/>
+      <c r="A93" s="14"/>
       <c r="B93" s="3" t="s">
         <v>185</v>
       </c>
@@ -15510,7 +15714,7 @@
       </c>
     </row>
     <row r="96" spans="1:21" ht="15" customHeight="1">
-      <c r="A96" s="15"/>
+      <c r="A96" s="14"/>
       <c r="B96" s="3" t="s">
         <v>191</v>
       </c>
@@ -15563,7 +15767,7 @@
       </c>
     </row>
     <row r="97" spans="1:21" ht="30">
-      <c r="A97" s="15"/>
+      <c r="A97" s="14"/>
       <c r="B97" s="3" t="s">
         <v>192</v>
       </c>
@@ -15618,7 +15822,7 @@
       </c>
     </row>
     <row r="98" spans="1:21" ht="15" customHeight="1">
-      <c r="A98" s="15"/>
+      <c r="A98" s="14"/>
       <c r="B98" s="4" t="s">
         <v>193</v>
       </c>
@@ -15673,7 +15877,7 @@
       </c>
     </row>
     <row r="99" spans="1:21" ht="45">
-      <c r="A99" s="15"/>
+      <c r="A99" s="14"/>
       <c r="B99" s="4" t="s">
         <v>194</v>
       </c>
@@ -15779,7 +15983,7 @@
       </c>
     </row>
     <row r="101" spans="1:21" ht="15" customHeight="1">
-      <c r="A101" s="15"/>
+      <c r="A101" s="14"/>
       <c r="B101" s="3" t="s">
         <v>196</v>
       </c>
@@ -15834,7 +16038,7 @@
       </c>
     </row>
     <row r="102" spans="1:21" ht="60">
-      <c r="A102" s="15"/>
+      <c r="A102" s="14"/>
       <c r="B102" s="3" t="s">
         <v>197</v>
       </c>
@@ -15889,7 +16093,7 @@
       </c>
     </row>
     <row r="103" spans="1:21" ht="15" customHeight="1">
-      <c r="A103" s="15"/>
+      <c r="A103" s="14"/>
       <c r="B103" s="4" t="s">
         <v>198</v>
       </c>
@@ -15944,7 +16148,7 @@
       </c>
     </row>
     <row r="104" spans="1:21" ht="30">
-      <c r="A104" s="15"/>
+      <c r="A104" s="14"/>
       <c r="B104" s="4" t="s">
         <v>199</v>
       </c>
@@ -15997,7 +16201,7 @@
       </c>
     </row>
     <row r="105" spans="1:21" ht="15" customHeight="1">
-      <c r="A105" s="15"/>
+      <c r="A105" s="14"/>
       <c r="B105" s="3" t="s">
         <v>200</v>
       </c>
@@ -16050,7 +16254,7 @@
       </c>
     </row>
     <row r="106" spans="1:21" ht="45">
-      <c r="A106" s="15"/>
+      <c r="A106" s="14"/>
       <c r="B106" s="4" t="s">
         <v>202</v>
       </c>
@@ -16154,7 +16358,7 @@
       </c>
     </row>
     <row r="108" spans="1:21" ht="15" customHeight="1">
-      <c r="A108" s="15"/>
+      <c r="A108" s="14"/>
       <c r="B108" s="3" t="s">
         <v>204</v>
       </c>
@@ -16205,7 +16409,7 @@
       </c>
     </row>
     <row r="109" spans="1:21" ht="60">
-      <c r="A109" s="15"/>
+      <c r="A109" s="14"/>
       <c r="B109" s="3" t="s">
         <v>206</v>
       </c>
@@ -16258,7 +16462,7 @@
       </c>
     </row>
     <row r="110" spans="1:21" ht="30">
-      <c r="A110" s="15"/>
+      <c r="A110" s="14"/>
       <c r="B110" s="4" t="s">
         <v>208</v>
       </c>
@@ -16311,7 +16515,7 @@
       </c>
     </row>
     <row r="111" spans="1:21" ht="15" customHeight="1">
-      <c r="A111" s="15"/>
+      <c r="A111" s="14"/>
       <c r="B111" s="4" t="s">
         <v>209</v>
       </c>
@@ -16362,7 +16566,7 @@
       </c>
     </row>
     <row r="112" spans="1:21" ht="30">
-      <c r="A112" s="15"/>
+      <c r="A112" s="14"/>
       <c r="B112" s="4" t="s">
         <v>211</v>
       </c>
@@ -16627,7 +16831,7 @@
       </c>
     </row>
     <row r="117" spans="1:21" ht="15" customHeight="1">
-      <c r="A117" s="15"/>
+      <c r="A117" s="14"/>
       <c r="B117" s="4" t="s">
         <v>220</v>
       </c>
@@ -16682,7 +16886,7 @@
       </c>
     </row>
     <row r="118" spans="1:21" ht="105">
-      <c r="A118" s="15"/>
+      <c r="A118" s="14"/>
       <c r="B118" s="4" t="s">
         <v>221</v>
       </c>
@@ -16841,7 +17045,7 @@
       </c>
     </row>
     <row r="121" spans="1:21" ht="15" customHeight="1">
-      <c r="A121" s="15"/>
+      <c r="A121" s="14"/>
       <c r="B121" s="4"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
@@ -16853,72 +17057,72 @@
       <c r="M121" s="4"/>
     </row>
     <row r="122" spans="1:21">
-      <c r="A122" s="15"/>
+      <c r="A122" s="14"/>
       <c r="I122" s="4"/>
       <c r="M122" s="4"/>
     </row>
     <row r="123" spans="1:21" ht="15" customHeight="1">
-      <c r="A123" s="15"/>
+      <c r="A123" s="14"/>
       <c r="I123" s="4"/>
       <c r="M123" s="4"/>
     </row>
     <row r="124" spans="1:21">
-      <c r="A124" s="15"/>
+      <c r="A124" s="14"/>
       <c r="I124" s="4"/>
       <c r="M124" s="4"/>
     </row>
     <row r="125" spans="1:21" ht="15" customHeight="1">
-      <c r="A125" s="15"/>
+      <c r="A125" s="14"/>
       <c r="I125" s="4"/>
       <c r="M125" s="4"/>
     </row>
     <row r="126" spans="1:21">
-      <c r="A126" s="15"/>
+      <c r="A126" s="14"/>
       <c r="I126" s="4"/>
       <c r="M126" s="4"/>
     </row>
     <row r="127" spans="1:21">
-      <c r="A127" s="15"/>
+      <c r="A127" s="14"/>
       <c r="I127" s="4"/>
       <c r="M127" s="4"/>
     </row>
     <row r="128" spans="1:21" ht="15" customHeight="1">
-      <c r="A128" s="15"/>
+      <c r="A128" s="14"/>
       <c r="I128" s="4"/>
       <c r="M128" s="4"/>
     </row>
     <row r="129" spans="1:13">
-      <c r="A129" s="15"/>
+      <c r="A129" s="14"/>
       <c r="I129" s="4"/>
       <c r="M129" s="4"/>
     </row>
     <row r="130" spans="1:13" ht="15" customHeight="1">
-      <c r="A130" s="15"/>
+      <c r="A130" s="14"/>
       <c r="I130" s="4"/>
       <c r="M130" s="4"/>
     </row>
     <row r="131" spans="1:13">
-      <c r="A131" s="15"/>
+      <c r="A131" s="14"/>
       <c r="I131" s="4"/>
       <c r="M131" s="4"/>
     </row>
     <row r="132" spans="1:13" ht="15" customHeight="1">
-      <c r="A132" s="15"/>
+      <c r="A132" s="14"/>
       <c r="I132" s="4"/>
       <c r="M132" s="4"/>
     </row>
     <row r="133" spans="1:13">
-      <c r="A133" s="15"/>
+      <c r="A133" s="14"/>
       <c r="I133" s="4"/>
       <c r="M133" s="4"/>
     </row>
     <row r="134" spans="1:13" ht="15" customHeight="1">
-      <c r="A134" s="15"/>
+      <c r="A134" s="14"/>
       <c r="I134" s="4"/>
       <c r="M134" s="4"/>
     </row>
     <row r="135" spans="1:13">
-      <c r="A135" s="15"/>
+      <c r="A135" s="14"/>
       <c r="I135" s="4"/>
       <c r="M135" s="4"/>
     </row>
@@ -16933,22 +17137,22 @@
       <c r="M137" s="4"/>
     </row>
     <row r="138" spans="1:13" ht="15" customHeight="1">
-      <c r="A138" s="15"/>
+      <c r="A138" s="14"/>
       <c r="I138" s="4"/>
       <c r="M138" s="4"/>
     </row>
     <row r="139" spans="1:13">
-      <c r="A139" s="15"/>
+      <c r="A139" s="14"/>
       <c r="I139" s="4"/>
       <c r="M139" s="4"/>
     </row>
     <row r="140" spans="1:13">
-      <c r="A140" s="15"/>
+      <c r="A140" s="14"/>
       <c r="I140" s="4"/>
       <c r="M140" s="4"/>
     </row>
     <row r="141" spans="1:13">
-      <c r="A141" s="15"/>
+      <c r="A141" s="14"/>
       <c r="I141" s="4"/>
       <c r="M141" s="4"/>
     </row>
@@ -16958,47 +17162,47 @@
       <c r="M142" s="4"/>
     </row>
     <row r="143" spans="1:13" ht="15" customHeight="1">
-      <c r="A143" s="15"/>
+      <c r="A143" s="14"/>
       <c r="I143" s="4"/>
       <c r="M143" s="4"/>
     </row>
     <row r="144" spans="1:13">
-      <c r="A144" s="15"/>
+      <c r="A144" s="14"/>
       <c r="I144" s="4"/>
       <c r="M144" s="4"/>
     </row>
     <row r="145" spans="1:13" ht="15" customHeight="1">
-      <c r="A145" s="15"/>
+      <c r="A145" s="14"/>
       <c r="I145" s="4"/>
       <c r="M145" s="4"/>
     </row>
     <row r="146" spans="1:13">
-      <c r="A146" s="15"/>
+      <c r="A146" s="14"/>
       <c r="I146" s="4"/>
       <c r="M146" s="4"/>
     </row>
     <row r="147" spans="1:13">
-      <c r="A147" s="15"/>
+      <c r="A147" s="14"/>
       <c r="I147" s="4"/>
       <c r="M147" s="4"/>
     </row>
     <row r="148" spans="1:13" ht="15" customHeight="1">
-      <c r="A148" s="15"/>
+      <c r="A148" s="14"/>
       <c r="I148" s="4"/>
       <c r="M148" s="4"/>
     </row>
     <row r="149" spans="1:13">
-      <c r="A149" s="15"/>
+      <c r="A149" s="14"/>
       <c r="I149" s="4"/>
       <c r="M149" s="4"/>
     </row>
     <row r="150" spans="1:13" ht="45" customHeight="1">
-      <c r="A150" s="15"/>
+      <c r="A150" s="14"/>
       <c r="I150" s="4"/>
       <c r="M150" s="4"/>
     </row>
     <row r="151" spans="1:13">
-      <c r="A151" s="15"/>
+      <c r="A151" s="14"/>
       <c r="I151" s="4"/>
       <c r="M151" s="4"/>
     </row>
@@ -17028,22 +17232,22 @@
       <c r="M156" s="4"/>
     </row>
     <row r="157" spans="1:13" ht="15" customHeight="1">
-      <c r="A157" s="15"/>
+      <c r="A157" s="14"/>
       <c r="I157" s="4"/>
       <c r="M157" s="4"/>
     </row>
     <row r="158" spans="1:13">
-      <c r="A158" s="15"/>
+      <c r="A158" s="14"/>
       <c r="I158" s="4"/>
       <c r="M158" s="4"/>
     </row>
     <row r="159" spans="1:13" ht="15" customHeight="1">
-      <c r="A159" s="15"/>
+      <c r="A159" s="14"/>
       <c r="I159" s="4"/>
       <c r="M159" s="4"/>
     </row>
     <row r="160" spans="1:13">
-      <c r="A160" s="15"/>
+      <c r="A160" s="14"/>
       <c r="I160" s="4"/>
       <c r="M160" s="4"/>
     </row>
@@ -17063,22 +17267,22 @@
       <c r="M163" s="4"/>
     </row>
     <row r="164" spans="1:13" ht="15" customHeight="1">
-      <c r="A164" s="15"/>
+      <c r="A164" s="14"/>
       <c r="I164" s="4"/>
       <c r="M164" s="4"/>
     </row>
     <row r="165" spans="1:13">
-      <c r="A165" s="15"/>
+      <c r="A165" s="14"/>
       <c r="I165" s="4"/>
       <c r="M165" s="4"/>
     </row>
     <row r="166" spans="1:13" ht="15" customHeight="1">
-      <c r="A166" s="15"/>
+      <c r="A166" s="14"/>
       <c r="I166" s="4"/>
       <c r="M166" s="4"/>
     </row>
     <row r="167" spans="1:13">
-      <c r="A167" s="15"/>
+      <c r="A167" s="14"/>
       <c r="I167" s="4"/>
       <c r="M167" s="4"/>
     </row>
@@ -17088,12 +17292,12 @@
       <c r="M168" s="4"/>
     </row>
     <row r="169" spans="1:13" ht="15" customHeight="1">
-      <c r="A169" s="15"/>
+      <c r="A169" s="14"/>
       <c r="I169" s="4"/>
       <c r="M169" s="4"/>
     </row>
     <row r="170" spans="1:13">
-      <c r="A170" s="15"/>
+      <c r="A170" s="14"/>
       <c r="I170" s="4"/>
       <c r="M170" s="4"/>
     </row>
@@ -17113,67 +17317,67 @@
       <c r="M173" s="4"/>
     </row>
     <row r="174" spans="1:13" ht="15" customHeight="1">
-      <c r="A174" s="15"/>
+      <c r="A174" s="14"/>
       <c r="I174" s="4"/>
       <c r="M174" s="4"/>
     </row>
     <row r="175" spans="1:13">
-      <c r="A175" s="15"/>
+      <c r="A175" s="14"/>
       <c r="I175" s="4"/>
       <c r="M175" s="4"/>
     </row>
     <row r="176" spans="1:13" ht="15" customHeight="1">
-      <c r="A176" s="15"/>
+      <c r="A176" s="14"/>
       <c r="I176" s="4"/>
       <c r="M176" s="4"/>
     </row>
     <row r="177" spans="1:13">
-      <c r="A177" s="15"/>
+      <c r="A177" s="14"/>
       <c r="I177" s="4"/>
       <c r="M177" s="4"/>
     </row>
     <row r="178" spans="1:13">
-      <c r="A178" s="15"/>
+      <c r="A178" s="14"/>
       <c r="I178" s="4"/>
       <c r="M178" s="4"/>
     </row>
     <row r="179" spans="1:13" ht="15" customHeight="1">
-      <c r="A179" s="15"/>
+      <c r="A179" s="14"/>
       <c r="I179" s="4"/>
       <c r="M179" s="4"/>
     </row>
     <row r="180" spans="1:13">
-      <c r="A180" s="15"/>
+      <c r="A180" s="14"/>
       <c r="I180" s="4"/>
       <c r="M180" s="4"/>
     </row>
     <row r="181" spans="1:13" ht="15" customHeight="1">
-      <c r="A181" s="15"/>
+      <c r="A181" s="14"/>
       <c r="I181" s="4"/>
       <c r="M181" s="4"/>
     </row>
     <row r="182" spans="1:13">
-      <c r="A182" s="15"/>
+      <c r="A182" s="14"/>
       <c r="I182" s="4"/>
       <c r="M182" s="4"/>
     </row>
     <row r="183" spans="1:13" ht="15" customHeight="1">
-      <c r="A183" s="15"/>
+      <c r="A183" s="14"/>
       <c r="I183" s="4"/>
       <c r="M183" s="4"/>
     </row>
     <row r="184" spans="1:13">
-      <c r="A184" s="15"/>
+      <c r="A184" s="14"/>
       <c r="I184" s="4"/>
       <c r="M184" s="4"/>
     </row>
     <row r="185" spans="1:13" ht="15" customHeight="1">
-      <c r="A185" s="15"/>
+      <c r="A185" s="14"/>
       <c r="I185" s="4"/>
       <c r="M185" s="4"/>
     </row>
     <row r="186" spans="1:13">
-      <c r="A186" s="15"/>
+      <c r="A186" s="14"/>
       <c r="I186" s="4"/>
       <c r="M186" s="4"/>
     </row>
@@ -17183,22 +17387,22 @@
       <c r="M187" s="4"/>
     </row>
     <row r="188" spans="1:13" ht="15" customHeight="1">
-      <c r="A188" s="15"/>
+      <c r="A188" s="14"/>
       <c r="I188" s="4"/>
       <c r="M188" s="4"/>
     </row>
     <row r="189" spans="1:13">
-      <c r="A189" s="15"/>
+      <c r="A189" s="14"/>
       <c r="I189" s="4"/>
       <c r="M189" s="4"/>
     </row>
     <row r="190" spans="1:13" ht="60" customHeight="1">
-      <c r="A190" s="15"/>
+      <c r="A190" s="14"/>
       <c r="I190" s="4"/>
       <c r="M190" s="4"/>
     </row>
     <row r="191" spans="1:13">
-      <c r="A191" s="15"/>
+      <c r="A191" s="14"/>
       <c r="I191" s="4"/>
       <c r="M191" s="4"/>
     </row>
@@ -17208,12 +17412,12 @@
       <c r="M192" s="4"/>
     </row>
     <row r="193" spans="1:13" ht="45" customHeight="1">
-      <c r="A193" s="15"/>
+      <c r="A193" s="14"/>
       <c r="I193" s="4"/>
       <c r="M193" s="4"/>
     </row>
     <row r="194" spans="1:13">
-      <c r="A194" s="15"/>
+      <c r="A194" s="14"/>
       <c r="I194" s="4"/>
       <c r="M194" s="4"/>
     </row>
@@ -17222,58 +17426,6 @@
     <sortCondition ref="T1:T232"/>
   </sortState>
   <mergeCells count="68">
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A79:A81"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A101:A102"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A108:A110"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="A145:A147"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="A138:A139"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="A193:A194"/>
     <mergeCell ref="A190:A191"/>
@@ -17290,6 +17442,58 @@
     <mergeCell ref="A159:A160"/>
     <mergeCell ref="A157:A158"/>
     <mergeCell ref="A150:A151"/>
+    <mergeCell ref="A148:A149"/>
+    <mergeCell ref="A145:A147"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A140:A141"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="A128:A129"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A108:A110"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="A88:A89"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A79:A81"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" tooltip="Absolute Zero" display="http://crawl.chaosforge.org/Absolute_Zero" xr:uid="{0B7D80AD-41C3-4378-86E9-351B477A2B9F}"/>
@@ -17480,7 +17684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E8B271-C60B-40E0-8071-44B09290B0A0}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -18666,10 +18870,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E9C651-19A5-494D-8095-C1365B59BB3C}">
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F78" sqref="F78"/>
+    <sheetView tabSelected="1" topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="L61" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18679,9 +18883,12 @@
     <col min="4" max="4" width="29.28515625" customWidth="1"/>
     <col min="5" max="5" width="55.28515625" customWidth="1"/>
     <col min="7" max="7" width="55.28515625" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>570</v>
       </c>
@@ -18697,8 +18904,17 @@
       <c r="G1" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" t="s">
+        <v>854</v>
+      </c>
+      <c r="K1" t="s">
+        <v>607</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>571</v>
       </c>
@@ -18716,8 +18932,22 @@
       <c r="G2" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="str">
+        <f>SUBSTITUTE(A2, "_", " ")</f>
+        <v>spit poison</v>
+      </c>
+      <c r="I2" t="s">
+        <v>855</v>
+      </c>
+      <c r="K2" t="s">
+        <v>608</v>
+      </c>
+      <c r="L2">
+        <f>L1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>572</v>
       </c>
@@ -18735,8 +18965,22 @@
       <c r="G3" t="s">
         <v>721</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:I66" si="2">SUBSTITUTE(A3, "_", " ")</f>
+        <v>blink</v>
+      </c>
+      <c r="I3" t="s">
+        <v>891</v>
+      </c>
+      <c r="K3" t="s">
+        <v>656</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L66" si="3">L2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>573</v>
       </c>
@@ -18754,8 +18998,22 @@
       <c r="G4" t="s">
         <v>677</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>flight</v>
+      </c>
+      <c r="I4" t="s">
+        <v>888</v>
+      </c>
+      <c r="K4" t="s">
+        <v>653</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>574</v>
       </c>
@@ -18773,8 +19031,22 @@
       <c r="G5" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>berserk</v>
+      </c>
+      <c r="I5" t="s">
+        <v>641</v>
+      </c>
+      <c r="K5" t="s">
+        <v>641</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>575</v>
       </c>
@@ -18792,8 +19064,22 @@
       <c r="G6" t="s">
         <v>685</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>hop</v>
+      </c>
+      <c r="I6" t="s">
+        <v>621</v>
+      </c>
+      <c r="K6" t="s">
+        <v>621</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>576</v>
       </c>
@@ -18811,8 +19097,22 @@
       <c r="G7" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>heal wounds</v>
+      </c>
+      <c r="I7" t="s">
+        <v>864</v>
+      </c>
+      <c r="K7" t="s">
+        <v>623</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>577</v>
       </c>
@@ -18830,8 +19130,22 @@
       <c r="G8" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>rolling charge</v>
+      </c>
+      <c r="I8" t="s">
+        <v>833</v>
+      </c>
+      <c r="K8" t="s">
+        <v>578</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>578</v>
       </c>
@@ -18849,8 +19163,22 @@
       <c r="G9" t="s">
         <v>698</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>bat form</v>
+      </c>
+      <c r="I9" t="s">
+        <v>863</v>
+      </c>
+      <c r="K9" t="s">
+        <v>620</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>579</v>
       </c>
@@ -18871,8 +19199,22 @@
       <c r="G10" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>curse item</v>
+      </c>
+      <c r="I10" t="s">
+        <v>837</v>
+      </c>
+      <c r="K10" t="s">
+        <v>586</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>580</v>
       </c>
@@ -18890,8 +19232,22 @@
       <c r="G11" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>scrying</v>
+      </c>
+      <c r="I11" t="s">
+        <v>574</v>
+      </c>
+      <c r="K11" t="s">
+        <v>574</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -18912,8 +19268,22 @@
       <c r="G12" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>transfer knowledge</v>
+      </c>
+      <c r="I12" t="s">
+        <v>572</v>
+      </c>
+      <c r="K12" t="s">
+        <v>572</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>582</v>
       </c>
@@ -18931,8 +19301,22 @@
       <c r="G13" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>smite</v>
+      </c>
+      <c r="I13" t="s">
+        <v>897</v>
+      </c>
+      <c r="K13" t="s">
+        <v>666</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>583</v>
       </c>
@@ -18950,8 +19334,22 @@
       <c r="G14" t="s">
         <v>761</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>recall</v>
+      </c>
+      <c r="I14" t="s">
+        <v>861</v>
+      </c>
+      <c r="K14" t="s">
+        <v>618</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>584</v>
       </c>
@@ -18969,8 +19367,22 @@
       <c r="G15" t="s">
         <v>720</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>give item to follower</v>
+      </c>
+      <c r="I15" t="s">
+        <v>848</v>
+      </c>
+      <c r="K15" t="s">
+        <v>600</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>585</v>
       </c>
@@ -18988,8 +19400,22 @@
       <c r="G16" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>resurrection</v>
+      </c>
+      <c r="I16" t="s">
+        <v>853</v>
+      </c>
+      <c r="K16" t="s">
+        <v>606</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>586</v>
       </c>
@@ -19007,8 +19433,22 @@
       <c r="G17" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>bend time</v>
+      </c>
+      <c r="I17" t="s">
+        <v>882</v>
+      </c>
+      <c r="K17" t="s">
+        <v>646</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>587</v>
       </c>
@@ -19026,8 +19466,22 @@
       <c r="G18" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>temporal distortion</v>
+      </c>
+      <c r="I18" t="s">
+        <v>852</v>
+      </c>
+      <c r="K18" t="s">
+        <v>605</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>588</v>
       </c>
@@ -19045,8 +19499,22 @@
       <c r="G19" t="s">
         <v>692</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>slouch</v>
+      </c>
+      <c r="I19" t="s">
+        <v>879</v>
+      </c>
+      <c r="K19" t="s">
+        <v>643</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>589</v>
       </c>
@@ -19064,8 +19532,22 @@
       <c r="G20" t="s">
         <v>760</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>step from time</v>
+      </c>
+      <c r="I20" t="s">
+        <v>895</v>
+      </c>
+      <c r="K20" t="s">
+        <v>664</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>590</v>
       </c>
@@ -19083,8 +19565,22 @@
       <c r="G21" t="s">
         <v>697</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>shadow step</v>
+      </c>
+      <c r="I21" t="s">
+        <v>845</v>
+      </c>
+      <c r="K21" t="s">
+        <v>596</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>591</v>
       </c>
@@ -19102,8 +19598,22 @@
       <c r="G22" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>shadow form</v>
+      </c>
+      <c r="I22" t="s">
+        <v>622</v>
+      </c>
+      <c r="K22" t="s">
+        <v>622</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>592</v>
       </c>
@@ -19121,8 +19631,22 @@
       <c r="G23" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>lesser healing</v>
+      </c>
+      <c r="I23" t="s">
+        <v>865</v>
+      </c>
+      <c r="K23" t="s">
+        <v>624</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>593</v>
       </c>
@@ -19140,8 +19664,22 @@
       <c r="G24" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>divine protection</v>
+      </c>
+      <c r="I24" t="s">
+        <v>858</v>
+      </c>
+      <c r="K24" t="s">
+        <v>614</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>594</v>
       </c>
@@ -19159,8 +19697,22 @@
       <c r="G25" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>heal other</v>
+      </c>
+      <c r="I25" t="s">
+        <v>834</v>
+      </c>
+      <c r="K25" t="s">
+        <v>579</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>596</v>
       </c>
@@ -19178,8 +19730,22 @@
       <c r="G26" t="s">
         <v>672</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>controlled blink</v>
+      </c>
+      <c r="I26" t="s">
+        <v>872</v>
+      </c>
+      <c r="K26" t="s">
+        <v>632</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>597</v>
       </c>
@@ -19197,8 +19763,22 @@
       <c r="G27" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>purification</v>
+      </c>
+      <c r="I27" t="s">
+        <v>862</v>
+      </c>
+      <c r="K27" t="s">
+        <v>619</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>598</v>
       </c>
@@ -19216,8 +19796,22 @@
       <c r="G28" t="s">
         <v>696</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>greater healing</v>
+      </c>
+      <c r="I28" t="s">
+        <v>875</v>
+      </c>
+      <c r="K28" t="s">
+        <v>638</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>599</v>
       </c>
@@ -19235,8 +19829,22 @@
       <c r="G29" t="s">
         <v>699</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>divine vigour</v>
+      </c>
+      <c r="I29" t="s">
+        <v>843</v>
+      </c>
+      <c r="K29" t="s">
+        <v>593</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>600</v>
       </c>
@@ -19254,8 +19862,22 @@
       <c r="G30" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>briar patch</v>
+      </c>
+      <c r="I30" t="s">
+        <v>894</v>
+      </c>
+      <c r="K30" t="s">
+        <v>663</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>601</v>
       </c>
@@ -19273,8 +19895,22 @@
       <c r="G31" t="s">
         <v>675</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>grow ballistomycete</v>
+      </c>
+      <c r="I31" t="s">
+        <v>847</v>
+      </c>
+      <c r="K31" t="s">
+        <v>599</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>602</v>
       </c>
@@ -19292,8 +19928,22 @@
       <c r="G32" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>overgrow</v>
+      </c>
+      <c r="I32" t="s">
+        <v>892</v>
+      </c>
+      <c r="K32" t="s">
+        <v>657</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>603</v>
       </c>
@@ -19311,8 +19961,22 @@
       <c r="G33" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>grow oklob plant</v>
+      </c>
+      <c r="I33" t="s">
+        <v>876</v>
+      </c>
+      <c r="K33" t="s">
+        <v>639</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>604</v>
       </c>
@@ -19333,8 +19997,22 @@
       <c r="G34" t="s">
         <v>708</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>potion petition</v>
+      </c>
+      <c r="I34" t="s">
+        <v>874</v>
+      </c>
+      <c r="K34" t="s">
+        <v>637</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>605</v>
       </c>
@@ -19352,8 +20030,22 @@
       <c r="G35" t="s">
         <v>691</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>call merchant</v>
+      </c>
+      <c r="I35" t="s">
+        <v>893</v>
+      </c>
+      <c r="K35" t="s">
+        <v>658</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>606</v>
       </c>
@@ -19371,8 +20063,22 @@
       <c r="G36" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>bribe branch</v>
+      </c>
+      <c r="I36" t="s">
+        <v>635</v>
+      </c>
+      <c r="K36" t="s">
+        <v>635</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>607</v>
       </c>
@@ -19393,8 +20099,22 @@
       <c r="G37" t="s">
         <v>682</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>ancestor identity</v>
+      </c>
+      <c r="I37" t="s">
+        <v>573</v>
+      </c>
+      <c r="K37" t="s">
+        <v>573</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>608</v>
       </c>
@@ -19415,8 +20135,22 @@
       <c r="G38" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>ancestor life</v>
+      </c>
+      <c r="I38" t="s">
+        <v>880</v>
+      </c>
+      <c r="K38" t="s">
+        <v>644</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>609</v>
       </c>
@@ -19434,8 +20168,22 @@
       <c r="G39" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>transference</v>
+      </c>
+      <c r="I39" t="s">
+        <v>857</v>
+      </c>
+      <c r="K39" t="s">
+        <v>612</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>610</v>
       </c>
@@ -19453,8 +20201,22 @@
       <c r="G40" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>idealise</v>
+      </c>
+      <c r="I40" t="s">
+        <v>836</v>
+      </c>
+      <c r="K40" t="s">
+        <v>584</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>611</v>
       </c>
@@ -19472,8 +20234,22 @@
       <c r="G41" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>request jelly</v>
+      </c>
+      <c r="I41" t="s">
+        <v>884</v>
+      </c>
+      <c r="K41" t="s">
+        <v>649</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>612</v>
       </c>
@@ -19491,8 +20267,22 @@
       <c r="G42" t="s">
         <v>709</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>gain random mutations</v>
+      </c>
+      <c r="I42" t="s">
+        <v>846</v>
+      </c>
+      <c r="K42" t="s">
+        <v>598</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>613</v>
       </c>
@@ -19510,8 +20300,22 @@
       <c r="G43" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>slimify</v>
+      </c>
+      <c r="I43" t="s">
+        <v>849</v>
+      </c>
+      <c r="K43" t="s">
+        <v>601</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>614</v>
       </c>
@@ -19529,8 +20333,22 @@
       <c r="G44" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>cure bad mutations</v>
+      </c>
+      <c r="I44" t="s">
+        <v>850</v>
+      </c>
+      <c r="K44" t="s">
+        <v>603</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>615</v>
       </c>
@@ -19548,8 +20366,22 @@
       <c r="G45" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>receive corpses</v>
+      </c>
+      <c r="I45" t="s">
+        <v>844</v>
+      </c>
+      <c r="K45" t="s">
+        <v>594</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>616</v>
       </c>
@@ -19567,8 +20399,22 @@
       <c r="G46" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>torment</v>
+      </c>
+      <c r="I46" t="s">
+        <v>831</v>
+      </c>
+      <c r="K46" t="s">
+        <v>576</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>617</v>
       </c>
@@ -19586,8 +20432,22 @@
       <c r="G47" t="s">
         <v>690</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>receive necronomicon</v>
+      </c>
+      <c r="I47" t="s">
+        <v>887</v>
+      </c>
+      <c r="K47" t="s">
+        <v>652</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>618</v>
       </c>
@@ -19608,8 +20468,22 @@
       <c r="G48" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>brand weapon with pain</v>
+      </c>
+      <c r="I48" t="s">
+        <v>634</v>
+      </c>
+      <c r="K48" t="s">
+        <v>634</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>619</v>
       </c>
@@ -19627,8 +20501,22 @@
       <c r="G49" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>depart abyss</v>
+      </c>
+      <c r="I49" t="s">
+        <v>575</v>
+      </c>
+      <c r="K49" t="s">
+        <v>575</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50" t="s">
         <v>620</v>
       </c>
@@ -19646,8 +20534,22 @@
       <c r="G50" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>bend space</v>
+      </c>
+      <c r="I50" t="s">
+        <v>610</v>
+      </c>
+      <c r="K50" t="s">
+        <v>610</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51" t="s">
         <v>621</v>
       </c>
@@ -19665,8 +20567,22 @@
       <c r="G51" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>banish</v>
+      </c>
+      <c r="I51" t="s">
+        <v>661</v>
+      </c>
+      <c r="K51" t="s">
+        <v>661</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52" t="s">
         <v>622</v>
       </c>
@@ -19684,8 +20600,22 @@
       <c r="G52" t="s">
         <v>762</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>corrupt</v>
+      </c>
+      <c r="I52" t="s">
+        <v>842</v>
+      </c>
+      <c r="K52" t="s">
+        <v>592</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53" t="s">
         <v>623</v>
       </c>
@@ -19703,8 +20633,22 @@
       <c r="G53" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>banish self</v>
+      </c>
+      <c r="I53" t="s">
+        <v>883</v>
+      </c>
+      <c r="K53" t="s">
+        <v>648</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54" t="s">
         <v>624</v>
       </c>
@@ -19725,8 +20669,22 @@
       <c r="G54" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>corrupt weapon</v>
+      </c>
+      <c r="I54" t="s">
+        <v>868</v>
+      </c>
+      <c r="K54" t="s">
+        <v>628</v>
+      </c>
+      <c r="L54">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55" t="s">
         <v>625</v>
       </c>
@@ -19744,8 +20702,22 @@
       <c r="G55" t="s">
         <v>686</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>minor destruction</v>
+      </c>
+      <c r="I55" t="s">
+        <v>866</v>
+      </c>
+      <c r="K55" t="s">
+        <v>625</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56" t="s">
         <v>627</v>
       </c>
@@ -19763,8 +20735,22 @@
       <c r="G56" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>summon lesser servant</v>
+      </c>
+      <c r="I56" t="s">
+        <v>602</v>
+      </c>
+      <c r="K56" t="s">
+        <v>602</v>
+      </c>
+      <c r="L56">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57" t="s">
         <v>628</v>
       </c>
@@ -19782,8 +20768,22 @@
       <c r="G57" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>major destruction</v>
+      </c>
+      <c r="I57" t="s">
+        <v>870</v>
+      </c>
+      <c r="K57" t="s">
+        <v>630</v>
+      </c>
+      <c r="L57">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58" t="s">
         <v>629</v>
       </c>
@@ -19801,8 +20801,22 @@
       <c r="G58" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>summon greater servant</v>
+      </c>
+      <c r="I58" t="s">
+        <v>851</v>
+      </c>
+      <c r="K58" t="s">
+        <v>604</v>
+      </c>
+      <c r="L58">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59" t="s">
         <v>630</v>
       </c>
@@ -19823,8 +20837,22 @@
       <c r="G59" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>pick a card any card</v>
+      </c>
+      <c r="I59" t="s">
+        <v>877</v>
+      </c>
+      <c r="K59" t="s">
+        <v>640</v>
+      </c>
+      <c r="L59">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60" t="s">
         <v>631</v>
       </c>
@@ -19845,8 +20873,22 @@
       <c r="G60" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>triple draw</v>
+      </c>
+      <c r="I60" t="s">
+        <v>597</v>
+      </c>
+      <c r="K60" t="s">
+        <v>597</v>
+      </c>
+      <c r="L60">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61" t="s">
         <v>632</v>
       </c>
@@ -19867,8 +20909,22 @@
       <c r="G61" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>deal four</v>
+      </c>
+      <c r="I61" t="s">
+        <v>583</v>
+      </c>
+      <c r="K61" t="s">
+        <v>583</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62" t="s">
         <v>633</v>
       </c>
@@ -19889,8 +20945,22 @@
       <c r="G62" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>stack five</v>
+      </c>
+      <c r="I62" t="s">
+        <v>890</v>
+      </c>
+      <c r="K62" t="s">
+        <v>655</v>
+      </c>
+      <c r="L62">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63" t="s">
         <v>634</v>
       </c>
@@ -19908,8 +20978,22 @@
       <c r="G63" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>heroism</v>
+      </c>
+      <c r="I63" t="s">
+        <v>859</v>
+      </c>
+      <c r="K63" t="s">
+        <v>615</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64" t="s">
         <v>635</v>
       </c>
@@ -19927,8 +21011,22 @@
       <c r="G64" t="s">
         <v>719</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>finesse</v>
+      </c>
+      <c r="I64" t="s">
+        <v>860</v>
+      </c>
+      <c r="K64" t="s">
+        <v>617</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" t="s">
         <v>636</v>
       </c>
@@ -19946,8 +21044,22 @@
       <c r="G65" t="s">
         <v>694</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>upheaval</v>
+      </c>
+      <c r="I65" t="s">
+        <v>659</v>
+      </c>
+      <c r="K65" t="s">
+        <v>659</v>
+      </c>
+      <c r="L65">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66" t="s">
         <v>637</v>
       </c>
@@ -19965,8 +21077,22 @@
       <c r="G66" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>elemental force</v>
+      </c>
+      <c r="I66" t="s">
+        <v>856</v>
+      </c>
+      <c r="K66" t="s">
+        <v>611</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67" t="s">
         <v>638</v>
       </c>
@@ -19974,18 +21100,32 @@
         <v>0</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D95" si="2">IF(C67="menu","target_ability_menu", IF(C67="text","target_ability_text_message", IF(B67,"target_ability_location", "non_target_ability") ) )</f>
+        <f t="shared" ref="D67:D95" si="4">IF(C67="menu","target_ability_menu", IF(C67="text","target_ability_text_message", IF(B67,"target_ability_location", "non_target_ability") ) )</f>
         <v>non_target_ability</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E95" si="3">CONCATENATE("(",D67," ", A67, ")")</f>
+        <f t="shared" ref="E67:E95" si="5">CONCATENATE("(",D67," ", A67, ")")</f>
         <v>(non_target_ability disaster_area)</v>
       </c>
       <c r="G67" t="s">
         <v>683</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" t="str">
+        <f t="shared" ref="H67:I95" si="6">SUBSTITUTE(A67, "_", " ")</f>
+        <v>disaster area</v>
+      </c>
+      <c r="I67" t="s">
+        <v>585</v>
+      </c>
+      <c r="K67" t="s">
+        <v>585</v>
+      </c>
+      <c r="L67">
+        <f t="shared" ref="L67:L94" si="7">L66+1</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68" t="s">
         <v>639</v>
       </c>
@@ -19993,18 +21133,32 @@
         <v>0</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability draw_out_power)</v>
       </c>
       <c r="G68" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" t="str">
+        <f t="shared" si="6"/>
+        <v>draw out power</v>
+      </c>
+      <c r="I68" t="s">
+        <v>832</v>
+      </c>
+      <c r="K68" t="s">
+        <v>577</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69" t="s">
         <v>640</v>
       </c>
@@ -20012,18 +21166,32 @@
         <v>1</v>
       </c>
       <c r="D69" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location power_leap)</v>
       </c>
       <c r="G69" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" t="str">
+        <f t="shared" si="6"/>
+        <v>power leap</v>
+      </c>
+      <c r="I69" t="s">
+        <v>662</v>
+      </c>
+      <c r="K69" t="s">
+        <v>662</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70" t="s">
         <v>641</v>
       </c>
@@ -20031,18 +21199,32 @@
         <v>0</v>
       </c>
       <c r="D70" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability apocalypse)</v>
       </c>
       <c r="G70" t="s">
         <v>674</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" t="str">
+        <f t="shared" si="6"/>
+        <v>apocalypse</v>
+      </c>
+      <c r="I70" t="s">
+        <v>580</v>
+      </c>
+      <c r="K70" t="s">
+        <v>580</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71" t="s">
         <v>642</v>
       </c>
@@ -20050,18 +21232,32 @@
         <v>0</v>
       </c>
       <c r="D71" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability toggle_divine_energy)</v>
       </c>
       <c r="G71" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" t="str">
+        <f t="shared" si="6"/>
+        <v>toggle divine energy</v>
+      </c>
+      <c r="I71" t="s">
+        <v>886</v>
+      </c>
+      <c r="K71" t="s">
+        <v>651</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72" t="s">
         <v>643</v>
       </c>
@@ -20069,18 +21265,32 @@
         <v>0</v>
       </c>
       <c r="D72" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability channel_magic)</v>
       </c>
       <c r="G72" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" t="str">
+        <f t="shared" si="6"/>
+        <v>channel magic</v>
+      </c>
+      <c r="I72" t="s">
+        <v>841</v>
+      </c>
+      <c r="K72" t="s">
+        <v>591</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73" t="s">
         <v>644</v>
       </c>
@@ -20091,18 +21301,32 @@
         <v>626</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_menu</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_menu forget_spell)</v>
       </c>
       <c r="G73" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" t="str">
+        <f t="shared" si="6"/>
+        <v>forget spell</v>
+      </c>
+      <c r="I73" t="s">
+        <v>840</v>
+      </c>
+      <c r="K73" t="s">
+        <v>590</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" t="s">
         <v>645</v>
       </c>
@@ -20110,18 +21334,32 @@
         <v>0</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability trogs_hand)</v>
       </c>
       <c r="G74" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" t="str">
+        <f t="shared" si="6"/>
+        <v>trogs hand</v>
+      </c>
+      <c r="I74" t="s">
+        <v>613</v>
+      </c>
+      <c r="K74" t="s">
+        <v>613</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" t="s">
         <v>646</v>
       </c>
@@ -20129,18 +21367,32 @@
         <v>0</v>
       </c>
       <c r="D75" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability brothers_in_arms)</v>
       </c>
       <c r="G75" t="s">
         <v>700</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" t="str">
+        <f t="shared" si="6"/>
+        <v>brothers in arms</v>
+      </c>
+      <c r="I75" t="s">
+        <v>588</v>
+      </c>
+      <c r="K75" t="s">
+        <v>588</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76" t="s">
         <v>647</v>
       </c>
@@ -20148,18 +21400,32 @@
         <v>0</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability stomp)</v>
       </c>
       <c r="G76" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" t="str">
+        <f t="shared" si="6"/>
+        <v>stomp</v>
+      </c>
+      <c r="I76" t="s">
+        <v>582</v>
+      </c>
+      <c r="K76" t="s">
+        <v>582</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77" t="s">
         <v>648</v>
       </c>
@@ -20167,18 +21433,32 @@
         <v>1</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location line_pass)</v>
       </c>
       <c r="G77" t="s">
         <v>676</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" t="str">
+        <f t="shared" si="6"/>
+        <v>line pass</v>
+      </c>
+      <c r="I77" t="s">
+        <v>830</v>
+      </c>
+      <c r="K77" t="s">
+        <v>571</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78" t="s">
         <v>649</v>
       </c>
@@ -20186,18 +21466,32 @@
         <v>1</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location grand_finale)</v>
       </c>
       <c r="G78" t="s">
         <v>689</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" t="str">
+        <f t="shared" si="6"/>
+        <v>grand finale</v>
+      </c>
+      <c r="I78" t="s">
+        <v>873</v>
+      </c>
+      <c r="K78" t="s">
+        <v>633</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79" t="s">
         <v>650</v>
       </c>
@@ -20205,18 +21499,32 @@
         <v>0</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability wall_jump)</v>
       </c>
       <c r="G79" t="s">
         <v>681</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" t="str">
+        <f t="shared" si="6"/>
+        <v>wall jump</v>
+      </c>
+      <c r="I79" t="s">
+        <v>839</v>
+      </c>
+      <c r="K79" t="s">
+        <v>589</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80" t="s">
         <v>651</v>
       </c>
@@ -20224,18 +21532,32 @@
         <v>0</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability serpents_lash)</v>
       </c>
       <c r="G80" t="s">
         <v>670</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80" t="str">
+        <f t="shared" si="6"/>
+        <v>serpents lash</v>
+      </c>
+      <c r="I80" t="s">
+        <v>647</v>
+      </c>
+      <c r="K80" t="s">
+        <v>647</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81" t="s">
         <v>652</v>
       </c>
@@ -20243,18 +21565,32 @@
         <v>0</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability heavenly_storm)</v>
       </c>
       <c r="G81" t="s">
         <v>707</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" t="str">
+        <f t="shared" si="6"/>
+        <v>heavenly storm</v>
+      </c>
+      <c r="I81" t="s">
+        <v>896</v>
+      </c>
+      <c r="K81" t="s">
+        <v>665</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82" t="s">
         <v>653</v>
       </c>
@@ -20262,18 +21598,32 @@
         <v>1</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location animate_remains)</v>
       </c>
       <c r="G82" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" t="str">
+        <f t="shared" si="6"/>
+        <v>animate remains</v>
+      </c>
+      <c r="I82" t="s">
+        <v>869</v>
+      </c>
+      <c r="K82" t="s">
+        <v>629</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="7"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83" t="s">
         <v>654</v>
       </c>
@@ -20281,18 +21631,32 @@
         <v>0</v>
       </c>
       <c r="D83" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability toggle_injury_mirror)</v>
       </c>
       <c r="G83" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" t="str">
+        <f t="shared" si="6"/>
+        <v>toggle injury mirror</v>
+      </c>
+      <c r="I83" t="s">
+        <v>867</v>
+      </c>
+      <c r="K83" t="s">
+        <v>627</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84" t="s">
         <v>655</v>
       </c>
@@ -20300,18 +21664,32 @@
         <v>0</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability recall_undead_slaves)</v>
       </c>
       <c r="G84" t="s">
         <v>706</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="H84" t="str">
+        <f t="shared" si="6"/>
+        <v>recall undead slaves</v>
+      </c>
+      <c r="I84" t="s">
+        <v>838</v>
+      </c>
+      <c r="K84" t="s">
+        <v>587</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85" t="s">
         <v>656</v>
       </c>
@@ -20319,18 +21697,32 @@
         <v>1</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location animate_dead)</v>
       </c>
       <c r="G85" t="s">
         <v>763</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" t="str">
+        <f t="shared" si="6"/>
+        <v>animate dead</v>
+      </c>
+      <c r="I85" t="s">
+        <v>878</v>
+      </c>
+      <c r="K85" t="s">
+        <v>642</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
       <c r="A86" t="s">
         <v>657</v>
       </c>
@@ -20338,18 +21730,32 @@
         <v>0</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability drain_life)</v>
       </c>
       <c r="G86" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" t="str">
+        <f t="shared" si="6"/>
+        <v>drain life</v>
+      </c>
+      <c r="I86" t="s">
+        <v>889</v>
+      </c>
+      <c r="K86" t="s">
+        <v>654</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
       <c r="A87" t="s">
         <v>658</v>
       </c>
@@ -20357,18 +21763,32 @@
         <v>1</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location enslave_soul)</v>
       </c>
       <c r="G87" t="s">
         <v>722</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="H87" t="str">
+        <f t="shared" si="6"/>
+        <v>enslave soul</v>
+      </c>
+      <c r="I87" t="s">
+        <v>616</v>
+      </c>
+      <c r="K87" t="s">
+        <v>616</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
       <c r="A88" t="s">
         <v>659</v>
       </c>
@@ -20376,18 +21796,32 @@
         <v>0</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability recite)</v>
       </c>
       <c r="G88" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" t="str">
+        <f t="shared" si="6"/>
+        <v>recite</v>
+      </c>
+      <c r="I88" t="s">
+        <v>835</v>
+      </c>
+      <c r="K88" t="s">
+        <v>581</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12">
       <c r="A89" t="s">
         <v>660</v>
       </c>
@@ -20395,18 +21829,32 @@
         <v>0</v>
       </c>
       <c r="D89" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability vitalisation)</v>
       </c>
       <c r="G89" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" t="str">
+        <f t="shared" si="6"/>
+        <v>vitalisation</v>
+      </c>
+      <c r="I89" t="s">
+        <v>609</v>
+      </c>
+      <c r="K89" t="s">
+        <v>609</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12">
       <c r="A90" t="s">
         <v>661</v>
       </c>
@@ -20414,18 +21862,32 @@
         <v>1</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_location</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_location Imprison)</v>
       </c>
       <c r="G90" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" t="str">
+        <f t="shared" si="6"/>
+        <v>Imprison</v>
+      </c>
+      <c r="I90" t="s">
+        <v>871</v>
+      </c>
+      <c r="K90" t="s">
+        <v>631</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12">
       <c r="A91" t="s">
         <v>662</v>
       </c>
@@ -20433,18 +21895,32 @@
         <v>0</v>
       </c>
       <c r="D91" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability sanctuary)</v>
       </c>
       <c r="G91" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" t="str">
+        <f t="shared" si="6"/>
+        <v>sanctuary</v>
+      </c>
+      <c r="I91" t="s">
+        <v>881</v>
+      </c>
+      <c r="K91" t="s">
+        <v>645</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="7"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
       <c r="A92" t="s">
         <v>663</v>
       </c>
@@ -20452,18 +21928,32 @@
         <v>0</v>
       </c>
       <c r="D92" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability divine_shield)</v>
       </c>
       <c r="G92" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" t="str">
+        <f t="shared" si="6"/>
+        <v>divine shield</v>
+      </c>
+      <c r="I92" t="s">
+        <v>636</v>
+      </c>
+      <c r="K92" t="s">
+        <v>636</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12">
       <c r="A93" t="s">
         <v>664</v>
       </c>
@@ -20471,18 +21961,32 @@
         <v>0</v>
       </c>
       <c r="D93" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability cleansing_flame)</v>
       </c>
       <c r="G93" t="s">
         <v>680</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" t="str">
+        <f t="shared" si="6"/>
+        <v>cleansing flame</v>
+      </c>
+      <c r="I93" t="s">
+        <v>660</v>
+      </c>
+      <c r="K93" t="s">
+        <v>660</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="7"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" t="s">
         <v>665</v>
       </c>
@@ -20490,18 +21994,32 @@
         <v>0</v>
       </c>
       <c r="D94" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>non_target_ability</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(non_target_ability summon_divine_warrior)</v>
       </c>
       <c r="G94" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" t="str">
+        <f t="shared" si="6"/>
+        <v>summon divine warrior</v>
+      </c>
+      <c r="I94" t="s">
+        <v>885</v>
+      </c>
+      <c r="K94" t="s">
+        <v>650</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12">
       <c r="A95" t="s">
         <v>666</v>
       </c>
@@ -20512,22 +22030,27 @@
         <v>626</v>
       </c>
       <c r="D95" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>target_ability_menu</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>(target_ability_menu brand_weapon_with_holy)</v>
       </c>
       <c r="G95" t="s">
         <v>702</v>
       </c>
+      <c r="H95" t="str">
+        <f t="shared" si="6"/>
+        <v>brand weapon with holy</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G95">
-    <sortCondition ref="G2:G95"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K1:K95">
+    <sortCondition ref="K1:K95"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>